<commit_message>
cleaning up source code and documentation
</commit_message>
<xml_diff>
--- a/documentation/PARAMS.xlsx
+++ b/documentation/PARAMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C58B7-F891-BE4D-A2D5-8915EE0EAB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F13795-7297-A04D-B0BE-7E02019A20D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="203">
   <si>
     <t>Parameter</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>log(3)/2</t>
-  </si>
-  <si>
-    <t>Logistic regression providing estimates for all years based on values from 2003, 2008, and 2014</t>
   </si>
   <si>
     <t xml:space="preserve">Logistic regression providing estimates for all years </t>
@@ -366,9 +363,6 @@
     <t>"In the absence of intervention, the rate of transmission of HIV from a mother living with HIV to her child during pregnancy, labour, delivery or breastfeeding ranges from 15% to 45%."</t>
   </si>
   <si>
-    <t>KDHS 2003, 2008, and 2014</t>
-  </si>
-  <si>
     <t>AIDSinfo</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>(from de Oliveira)</t>
   </si>
   <si>
-    <t>(from DHS/Mojola)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Varies by age, sex, and year
 </t>
   </si>
@@ -471,12 +462,6 @@
   <si>
     <t>Lognormal
 Arrives at this value in 2003, constant after</t>
-  </si>
-  <si>
-    <t>Relative risk of transmission in all age groups other than 30-39 vs 30-39; female</t>
-  </si>
-  <si>
-    <t>Relative risk of transmission in all age groups other than 30-39 vs 30-39; male</t>
   </si>
   <si>
     <t>Country-specific deaths data (UN)</t>
@@ -601,29 +586,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t xml:space="preserve">See testing_projection.R </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Calculated using proportion receiving a test in the past 12 months; forecasted for all years and older age groups based on regressing on age and year
-(e.g., rate of 2 means people tested twice a year; rate of 0.5 means tested every two years)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
       <t>See age_mixing.R</t>
     </r>
     <r>
@@ -794,14 +756,146 @@
     <t>Probability calculated from deaths data; projected using regression</t>
   </si>
   <si>
+    <t>Might have age/sex data for South Africa</t>
+  </si>
+  <si>
+    <t>Calculated as a regression fit to deaths data from 1950-1987 and 2008-2019 (to remove AIDS and COVID deaths)
+Log linear model - for each stratum of age*sex, fit the model: 
+fit = lm(log(rates) ~ years)
+Then projected until 2040</t>
+  </si>
+  <si>
+    <t>Consider making the regression a spline instead of only for select years - different slope post-spline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45-64 general mortality INTERCEPT multiplier, male </t>
+  </si>
+  <si>
+    <t>45-64 general mortality SLOPE multiplier, male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65-79 general mortality INTERCEPT multiplier, male </t>
+  </si>
+  <si>
+    <t>65-79 general mortality SLOPE multiplier, male</t>
+  </si>
+  <si>
+    <t>80+ general mortality INTERCEPT multiplier, male</t>
+  </si>
+  <si>
+    <t>80+ general mortality SLOPE multiplier, male</t>
+  </si>
+  <si>
+    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 45-64, male</t>
+  </si>
+  <si>
+    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 45-64, male</t>
+  </si>
+  <si>
+    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 65-79, male</t>
+  </si>
+  <si>
+    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 65-79, male</t>
+  </si>
+  <si>
+    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 80+, male</t>
+  </si>
+  <si>
+    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 80+, male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45-64 general mortality INTERCEPT multiplier, female </t>
+  </si>
+  <si>
+    <t>45-64 general mortality SLOPE multiplier, female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65-79 general mortality INTERCEPT multiplier, female </t>
+  </si>
+  <si>
+    <t>65-79 general mortality SLOPE multiplier, female</t>
+  </si>
+  <si>
+    <t>80+ general mortality INTERCEPT multiplier, female</t>
+  </si>
+  <si>
+    <t>80+ general mortality SLOPE multiplier, female</t>
+  </si>
+  <si>
+    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 45-64, female</t>
+  </si>
+  <si>
+    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 45-64, female</t>
+  </si>
+  <si>
+    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 65-79, female</t>
+  </si>
+  <si>
+    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 65-79, female</t>
+  </si>
+  <si>
+    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 80+, female</t>
+  </si>
+  <si>
+    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 80+, female</t>
+  </si>
+  <si>
+    <t>1
+Lognormal
+2 separate multipliers at HIV mortality times: 2005, 2030</t>
+  </si>
+  <si>
+    <t>1
+Lognormal
+Split up youngest age group into 0-4 and 5-14 in 1990 only</t>
+  </si>
+  <si>
+    <t>0-4 HIV-specific mortality multiplier, 1990</t>
+  </si>
+  <si>
+    <t>0-14 HIV-specific mortality</t>
+  </si>
+  <si>
+    <t>15-24 HIV-specific mortality</t>
+  </si>
+  <si>
+    <t>50+ HIV-specific mortality</t>
+  </si>
+  <si>
+    <t>5-14 HIV-specific mortality multiplier, 1990</t>
+  </si>
+  <si>
+    <t>Relative risk of transmission by age group, female</t>
+  </si>
+  <si>
+    <t>(same as female)</t>
+  </si>
+  <si>
+    <t>Relative risk of transmission by age group, male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See country-specific notes and  transmission_multipliers.R in each parameter_mappings/country folder; each of these calculated as some probability of high-risk sex; relative to a reference age group </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(same as female) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ages &lt;50: SABSSM 2012 (Tables 3.38-41), 2017 (Tables 3.45-47), 2022 Summary (Figues IX-X), 2022 Summary Sheet (pg 5) 
+Ages 50-80: Mojola et al, 2015 </t>
+  </si>
+  <si>
+    <t>KDHS 2003 (Table 12.10), 2008 (Tables 13.9.1-2), and 2014 (Tables 13.12.1-2)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>See age_sex_transmission_multipliers.R</t>
+      <t xml:space="preserve">Years </t>
     </r>
     <r>
       <rPr>
@@ -812,129 +906,230 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-(proportion with multiple partners or proportion high risk sex)* (proportion of condomless sex); converted to multiplier relative to reference age (30-39)</t>
+- DHS: 2003, 2008, 2014
+</t>
     </r>
-  </si>
-  <si>
-    <t>Might have age/sex data for South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allison found estimates of multiple partners and condom use by age (15-24, 25-49, 50+) in South African National HIV Prevalence, Incidence and Behaviour Surveys; Mojola is actually a SA paper so can use that for 50+ </t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t>Allison found estimate of % tested in the past year from South African National HIV Prevalence, Incidence and Behaviour Survey - just by sex; will also probably have to multiply by % ever tested; 2022 report has 15-24, 25-49, 50+ not by sex and only tested in the past 3 years</t>
-  </si>
-  <si>
-    <t>SABSSM</t>
-  </si>
-  <si>
-    <t>Calculated as a regression fit to deaths data from 1950-1987 and 2008-2019 (to remove AIDS and COVID deaths)
-Log linear model - for each stratum of age*sex, fit the model: 
-fit = lm(log(rates) ~ years)
-Then projected until 2040</t>
-  </si>
-  <si>
-    <t>Consider making the regression a spline instead of only for select years - different slope post-spline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45-64 general mortality INTERCEPT multiplier, male </t>
-  </si>
-  <si>
-    <t>45-64 general mortality SLOPE multiplier, male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65-79 general mortality INTERCEPT multiplier, male </t>
-  </si>
-  <si>
-    <t>65-79 general mortality SLOPE multiplier, male</t>
-  </si>
-  <si>
-    <t>80+ general mortality INTERCEPT multiplier, male</t>
-  </si>
-  <si>
-    <t>80+ general mortality SLOPE multiplier, male</t>
-  </si>
-  <si>
-    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 45-64, male</t>
-  </si>
-  <si>
-    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 45-64, male</t>
-  </si>
-  <si>
-    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 65-79, male</t>
-  </si>
-  <si>
-    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 65-79, male</t>
-  </si>
-  <si>
-    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 80+, male</t>
-  </si>
-  <si>
-    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 80+, male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45-64 general mortality INTERCEPT multiplier, female </t>
-  </si>
-  <si>
-    <t>45-64 general mortality SLOPE multiplier, female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65-79 general mortality INTERCEPT multiplier, female </t>
-  </si>
-  <si>
-    <t>65-79 general mortality SLOPE multiplier, female</t>
-  </si>
-  <si>
-    <t>80+ general mortality INTERCEPT multiplier, female</t>
-  </si>
-  <si>
-    <t>80+ general mortality SLOPE multiplier, female</t>
-  </si>
-  <si>
-    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 45-64, female</t>
-  </si>
-  <si>
-    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 45-64, female</t>
-  </si>
-  <si>
-    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 65-79, female</t>
-  </si>
-  <si>
-    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 65-79, female</t>
-  </si>
-  <si>
-    <t>Multiplier for the INTERCEPT of the regression model fit to smooth/forecast mortality for age 80+, female</t>
-  </si>
-  <si>
-    <t>Multiplier for the SLOPE of the regression model fit to smooth/forecast mortality for age 80+, female</t>
-  </si>
-  <si>
-    <t>1
-Lognormal
-2 separate multipliers at HIV mortality times: 2005, 2030</t>
-  </si>
-  <si>
-    <t>1
-Lognormal
-Split up youngest age group into 0-4 and 5-14 in 1990 only</t>
-  </si>
-  <si>
-    <t>0-4 HIV-specific mortality multiplier, 1990</t>
-  </si>
-  <si>
-    <t>0-14 HIV-specific mortality</t>
-  </si>
-  <si>
-    <t>15-24 HIV-specific mortality</t>
-  </si>
-  <si>
-    <t>50+ HIV-specific mortality</t>
-  </si>
-  <si>
-    <t>5-14 HIV-specific mortality multiplier, 1990</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Age groups </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DHS: 15-19, 20-24, 25-29, 30-39, 40-49
+Percentage who have been tested for HIV in past 12 months and received result </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ages &lt;50: SA DHS 2003 (Table 5.13), 2016 (Tables 12.2.1-2) 
+Ages &lt;50: SABSSM 2012 (Tables 3.38-41), 2017 (Tables 3.45-47), 2022 Summary (Figues IX-X), 2022 Summary Sheet (pg 5) 
+Ages 50-80: Mojola et al, 2015 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Years </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DHS: 2003, 2008, 2014
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Age groups </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DHS: 15-19, 20-24, 25-29, 30-39, 40-49; reference age= 30-39
+- Mojola et al: 40-49, 50-59, 60-69, 70-79; reference age = 40-49
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DHS: (proportion with multiple partners or proportion high risk sex)* (proportion of condomless sex at last high risk sex)
+- Mojola: (proportion high risk sex)*(1-condom use among high risk sex) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Years
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- SABSSM: 2002, 2005, 2008, 2012, 2017
+- DHS: 2003, 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Age groups</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- SABSSM: 15-24, 25-49, 50+; reference age = 25-49
+- DHS: 15-19, 20-24, 25-29, 30-39, 40-49; reference age= 30-39 
+- Mojola et al: 40-49, 50-59, 60-69, 70-79; reference age = 40-49
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Calculation: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- SABSSM: (proportion with multiple partners)*(proportion sometimes or never condom use) 
+- DHS: (proportion with multiple partners or proportion high risk sex)* (proportion of condomless sex at last high risk sex)
+- Mojola: (proportion high risk sex)*(1-condom use among high risk sex)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Years </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DHS: 2003, 2008, 2016
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Age groups </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DHS: 15-19, 20-24, 25-29, 30-39, 40-49
+Percentage who have been tested for HIV in past 12 months and received result </t>
+    </r>
+  </si>
+  <si>
+    <t>SA DHS 2003 (Table 5.6), 2016 (Tables 12.4.1-2)</t>
+  </si>
+  <si>
+    <t>Generate parameter table using "get_testing_projection_and_param_table.R"
+See country-specific notes and  testing_projection.R in each parameter_mappings/country folder; logistic regression based on proportion receiving a test  in the past 12 months;  forecasted for all years and older age groups based on regressing on age and year
+(e.g., rate of 2 means people tested twice a year; rate of 0.5 means tested every two years)</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1362,6 +1557,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1728,10 +1932,10 @@
   <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,14 +1944,15 @@
     <col min="2" max="2" width="17.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="32.1640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="5" customWidth="1"/>
-    <col min="8" max="9" width="22" style="5" customWidth="1"/>
+    <col min="5" max="5" width="37.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="55" style="5" customWidth="1"/>
+    <col min="7" max="8" width="60.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="5" customWidth="1"/>
     <col min="10" max="10" width="17" style="5" customWidth="1"/>
     <col min="11" max="11" width="24" style="5" customWidth="1"/>
     <col min="12" max="12" width="26" style="5" customWidth="1"/>
-    <col min="13" max="14" width="24" style="5" customWidth="1"/>
+    <col min="13" max="13" width="37.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="24" style="5" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
@@ -1756,25 +1961,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="35"/>
       <c r="H1" s="35"/>
       <c r="I1" s="37"/>
       <c r="J1" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K1" s="43" t="s">
         <v>1</v>
@@ -1790,56 +1995,56 @@
       <c r="D2" s="42"/>
       <c r="E2" s="38"/>
       <c r="F2" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="I2" s="40" t="s">
         <v>28</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>29</v>
       </c>
       <c r="J2" s="39"/>
       <c r="K2" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="N2" s="40" t="s">
         <v>28</v>
-      </c>
-      <c r="N2" s="40" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="211" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" s="26"/>
       <c r="K3" s="26" t="s">
@@ -1860,17 +2065,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
@@ -1891,30 +2096,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="255" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>114</v>
+        <v>189</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>163</v>
+        <v>53</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="60" t="s">
+        <v>199</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="30" t="s">
@@ -1922,37 +2127,35 @@
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="N5" s="32"/>
     </row>
-    <row r="6" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>115</v>
+        <v>191</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>161</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E6" s="27"/>
       <c r="F6" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="I6" s="31"/>
       <c r="J6" s="30" t="s">
@@ -1960,35 +2163,35 @@
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="N6" s="32"/>
     </row>
     <row r="7" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="51" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="30" t="s">
@@ -2009,26 +2212,26 @@
     </row>
     <row r="8" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="51" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="30" t="s">
@@ -2049,26 +2252,26 @@
     </row>
     <row r="9" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="51" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="30" t="s">
@@ -2089,26 +2292,26 @@
     </row>
     <row r="10" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="51" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="30" t="s">
@@ -2127,24 +2330,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -2153,7 +2356,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
@@ -2164,25 +2367,25 @@
         <v>7</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I12" s="31"/>
       <c r="J12" s="30" t="s">
@@ -2190,31 +2393,31 @@
       </c>
       <c r="K12" s="20"/>
       <c r="L12" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="M12" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="N12" s="32"/>
     </row>
     <row r="13" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
@@ -2235,25 +2438,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
@@ -2262,29 +2465,29 @@
       </c>
       <c r="K14" s="20"/>
       <c r="L14" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M14" s="31"/>
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
@@ -2293,32 +2496,32 @@
         <v>9</v>
       </c>
       <c r="K15" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M15" s="27"/>
       <c r="N15" s="29"/>
     </row>
     <row r="16" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
@@ -2327,7 +2530,7 @@
         <v>5</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
@@ -2335,22 +2538,22 @@
     </row>
     <row r="17" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="51"/>
@@ -2373,22 +2576,22 @@
     </row>
     <row r="18" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="51"/>
@@ -2411,22 +2614,22 @@
     </row>
     <row r="19" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="51"/>
@@ -2449,22 +2652,22 @@
     </row>
     <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="51"/>
@@ -2487,22 +2690,22 @@
     </row>
     <row r="21" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="51"/>
@@ -2525,22 +2728,22 @@
     </row>
     <row r="22" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="51"/>
@@ -2563,22 +2766,22 @@
     </row>
     <row r="23" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="51"/>
@@ -2601,22 +2804,22 @@
     </row>
     <row r="24" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="51"/>
@@ -2639,22 +2842,22 @@
     </row>
     <row r="25" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="51"/>
@@ -2677,22 +2880,22 @@
     </row>
     <row r="26" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="51"/>
@@ -2715,22 +2918,22 @@
     </row>
     <row r="27" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="51"/>
@@ -2753,22 +2956,22 @@
     </row>
     <row r="28" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="51"/>
@@ -2791,22 +2994,22 @@
     </row>
     <row r="29" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -2815,7 +3018,7 @@
         <v>3</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
@@ -2823,20 +3026,20 @@
     </row>
     <row r="30" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -2846,27 +3049,27 @@
       </c>
       <c r="K30" s="16"/>
       <c r="L30" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M30" s="14"/>
       <c r="N30" s="15"/>
     </row>
     <row r="31" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -2876,27 +3079,27 @@
       </c>
       <c r="K31" s="16"/>
       <c r="L31" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M31" s="14"/>
       <c r="N31" s="15"/>
     </row>
     <row r="32" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
@@ -2919,20 +3122,20 @@
     </row>
     <row r="33" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -2955,20 +3158,20 @@
     </row>
     <row r="34" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
@@ -2991,20 +3194,20 @@
     </row>
     <row r="35" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -3027,20 +3230,20 @@
     </row>
     <row r="36" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
@@ -3061,22 +3264,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A37" s="44" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D37" s="47"/>
       <c r="E37" s="45" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F37" s="44" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
@@ -3085,7 +3288,7 @@
         <v>5</v>
       </c>
       <c r="K37" s="52" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="L37" s="36"/>
       <c r="M37" s="36"/>
@@ -3093,22 +3296,22 @@
     </row>
     <row r="38" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E38" s="45" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F38" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
@@ -3129,68 +3332,68 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="170" x14ac:dyDescent="0.2">
       <c r="A39" s="44" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D39" s="47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="45" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F39" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
       <c r="I39" s="18"/>
       <c r="J39" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="N39" s="45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="M39" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="N39" s="45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="119" x14ac:dyDescent="0.2">
-      <c r="A40" s="44" t="s">
+      <c r="B40" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="45" t="s">
-        <v>25</v>
-      </c>
       <c r="F40" s="44" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G40" s="44">
         <v>0.25</v>
       </c>
       <c r="H40" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I40" s="44"/>
       <c r="J40" s="48" t="s">
@@ -3211,26 +3414,26 @@
     </row>
     <row r="41" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E41" s="45"/>
       <c r="F41" s="44" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G41" s="44">
         <v>0.25</v>
       </c>
       <c r="H41" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I41" s="44"/>
       <c r="J41" s="48" t="s">
@@ -3251,26 +3454,26 @@
     </row>
     <row r="42" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D42" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E42" s="45"/>
       <c r="F42" s="44" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G42" s="44">
         <v>2</v>
       </c>
       <c r="H42" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I42" s="44"/>
       <c r="J42" s="48" t="s">
@@ -3291,26 +3494,26 @@
     </row>
     <row r="43" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="46" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D43" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E43" s="45"/>
       <c r="F43" s="44" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G43" s="44">
         <v>2</v>
       </c>
       <c r="H43" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I43" s="44"/>
       <c r="J43" s="48" t="s">
@@ -3331,26 +3534,26 @@
     </row>
     <row r="44" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D44" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E44" s="45"/>
       <c r="F44" s="44" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G44" s="44">
         <v>2</v>
       </c>
       <c r="H44" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I44" s="44"/>
       <c r="J44" s="48" t="s">
@@ -3371,30 +3574,30 @@
     </row>
     <row r="45" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D45" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E45" s="45"/>
       <c r="F45" s="44" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G45" s="44">
         <v>1</v>
       </c>
       <c r="H45" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I45" s="44"/>
       <c r="J45" s="48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K45" s="48" t="s">
         <v>2</v>
@@ -3409,30 +3612,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="276" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="31" t="s">
-        <v>165</v>
+        <v>107</v>
+      </c>
+      <c r="G46" s="62" t="s">
+        <v>196</v>
+      </c>
+      <c r="H46" s="60" t="s">
+        <v>200</v>
       </c>
       <c r="I46" s="31"/>
       <c r="J46" s="8" t="s">
@@ -3440,31 +3643,31 @@
       </c>
       <c r="K46" s="20"/>
       <c r="L46" s="6" t="s">
-        <v>81</v>
+        <v>195</v>
       </c>
       <c r="M46" s="31" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="N46" s="32"/>
     </row>
     <row r="47" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
@@ -3487,22 +3690,22 @@
     </row>
     <row r="48" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -3525,25 +3728,25 @@
     </row>
     <row r="49" spans="1:14" ht="214" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H49" s="31"/>
       <c r="I49" s="31"/>
@@ -3552,33 +3755,33 @@
       </c>
       <c r="K49" s="20"/>
       <c r="L49" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M49" s="31"/>
       <c r="N49" s="32"/>
     </row>
     <row r="50" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G50" s="18"/>
       <c r="H50" s="58" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I50" s="18"/>
       <c r="J50" s="8" t="s">
@@ -3599,26 +3802,26 @@
     </row>
     <row r="51" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G51" s="18"/>
       <c r="H51" s="58" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I51" s="18"/>
       <c r="J51" s="8" t="s">
@@ -3639,26 +3842,26 @@
     </row>
     <row r="52" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G52" s="18"/>
       <c r="H52" s="58" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I52" s="18"/>
       <c r="J52" s="8" t="s">
@@ -3679,26 +3882,26 @@
     </row>
     <row r="53" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C53" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="F53" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G53" s="18"/>
       <c r="H53" s="58" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I53" s="18"/>
       <c r="J53" s="8" t="s">
@@ -3719,22 +3922,22 @@
     </row>
     <row r="54" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G54" s="6">
         <v>0.1392621</v>
@@ -3746,27 +3949,27 @@
       </c>
       <c r="K54" s="20"/>
       <c r="L54" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M54" s="31"/>
       <c r="N54" s="32"/>
     </row>
     <row r="55" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G55" s="6">
         <v>0.1025866</v>
@@ -3778,33 +3981,33 @@
       </c>
       <c r="K55" s="20"/>
       <c r="L55" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M55" s="31"/>
       <c r="N55" s="32"/>
     </row>
     <row r="56" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G56" s="6">
         <v>0.67328849999999996</v>
       </c>
       <c r="H56" s="31" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I56" s="31"/>
       <c r="J56" s="8" t="s">
@@ -3812,27 +4015,27 @@
       </c>
       <c r="K56" s="20"/>
       <c r="L56" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M56" s="31"/>
       <c r="N56" s="32"/>
     </row>
     <row r="57" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G57" s="6">
         <v>0.67328849999999996</v>
@@ -3844,27 +4047,27 @@
       </c>
       <c r="K57" s="20"/>
       <c r="L57" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M57" s="31"/>
       <c r="N57" s="32"/>
     </row>
     <row r="58" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G58" s="6">
         <v>0.1971601</v>
@@ -3876,31 +4079,31 @@
       </c>
       <c r="K58" s="20"/>
       <c r="L58" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M58" s="31"/>
       <c r="N58" s="32"/>
     </row>
     <row r="59" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I59" s="18"/>
       <c r="J59" s="8" t="s">
@@ -3921,24 +4124,24 @@
     </row>
     <row r="60" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G60" s="18"/>
       <c r="H60" s="51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I60" s="18"/>
       <c r="J60" s="8" t="s">
@@ -3959,28 +4162,28 @@
     </row>
     <row r="61" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G61" s="18"/>
       <c r="H61" s="51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I61" s="18"/>
       <c r="J61" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K61" s="8" t="s">
         <v>2</v>
@@ -3997,46 +4200,46 @@
     </row>
     <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding uganda (part 2)
</commit_message>
<xml_diff>
--- a/documentation/PARAMS.xlsx
+++ b/documentation/PARAMS.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0F903A-C2A2-204D-BE4A-FCD65644B942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86043F77-F371-5C46-8E56-4B9630922BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="34040" windowHeight="19540" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$P$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$Q$59</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,10 +43,9 @@
   <authors>
     <author>tc={04385ABF-366F-F14D-B686-003B7FD6A102}</author>
     <author>tc={51F972CD-9F3E-FF43-98B5-159579D7B474}</author>
-    <author>tc={41F30597-8EA5-6B4E-BC92-48BBEE4F0910}</author>
   </authors>
   <commentList>
-    <comment ref="N14" authorId="0" shapeId="0" xr:uid="{04385ABF-366F-F14D-B686-003B7FD6A102}">
+    <comment ref="O14" authorId="0" shapeId="0" xr:uid="{04385ABF-366F-F14D-B686-003B7FD6A102}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -54,7 +53,7 @@
     This includes 13 prospective studies from different regions; 0.42 estimate was Kenya-specific but they have Europe, France specifically, and other African countries</t>
       </text>
     </comment>
-    <comment ref="M15" authorId="1" shapeId="0" xr:uid="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
+    <comment ref="N15" authorId="1" shapeId="0" xr:uid="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -62,20 +61,12 @@
     Update to WHO reference because this is actually a global estimate</t>
       </text>
     </comment>
-    <comment ref="G49" authorId="2" shapeId="0" xr:uid="{41F30597-8EA5-6B4E-BC92-48BBEE4F0910}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Consider using IeDEA data for Kenya as well and fit a similar model</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="222">
   <si>
     <t>Parameter</t>
   </si>
@@ -746,82 +737,6 @@
 Log linear model, fit the model: 
 fit = glm(log(prop) ~ year), for age &lt;17
 fit = glm(log(prop) ~ year + age + year:age), for age 18+</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">AIDS Info: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">data on # PWH on ART (calculated # starting each year)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Years:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2011-2021
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ages:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Total only
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Calculated using the total number of individuals starting ART/those off of ART
-Log linear model, fit the model: 
-fit = glm(log(prop) ~ year)</t>
     </r>
   </si>
   <si>
@@ -1448,16 +1363,105 @@
     <t>DHS 2004, 2010, 2022 (also have 1996, 1999) - see "DHS_tables.xlsx"</t>
   </si>
   <si>
-    <t>Using SOUTH AFRICA suppression data (IeDEA dashboard values suppressed for Tanzania; for the few values that are there, they look closer to SA's data than Kenya)</t>
-  </si>
-  <si>
-    <t>Using SA suppression data (IeDEA dashboard values suppressed for Tanz); values look closer to SA than Kenya</t>
-  </si>
-  <si>
     <t>IeDEA Dashboard</t>
   </si>
   <si>
     <t>IeDEA dashboard</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Using SOUTH AFRICA suppression data (IeDEA dashboard values mostly NA for Tanzania; for the few values that are there, they look closer to SA's data than Kenya)</t>
+  </si>
+  <si>
+    <t>Using SA suppression data (IeDEA dashboard values mostly NA for Tanz); values look closer to SA than Kenya</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">***3/25 switched to IeDEA method***
+AIDS Info: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">data on # PWH on ART (calculated # starting each year)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Years:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2011-2021
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ages:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Total only
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculated using the total number of individuals starting ART/those off of ART
+Log linear model, fit the model: 
+fit = glm(log(prop) ~ year)</t>
+    </r>
+  </si>
+  <si>
+    <t>Using SOUTH AFRICA suppression data (IeDEA dashboard values mostly NA for Uganda; for the few values that are there, they look closer to SA's data than Kenya)</t>
+  </si>
+  <si>
+    <t>Using SA suppression data (IeDEA dashboard values mostly NA for Uganda); values look closer to SA than Kenya</t>
+  </si>
+  <si>
+    <t>DHS 2000 2006, 2016 (also have 1995, 2011) - see "DHS_tables.xlsx"</t>
   </si>
 </sst>
 </file>
@@ -2268,27 +2272,24 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="N14" dT="2025-01-22T18:42:38.64" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{04385ABF-366F-F14D-B686-003B7FD6A102}">
+  <threadedComment ref="O14" dT="2025-01-22T18:42:38.64" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{04385ABF-366F-F14D-B686-003B7FD6A102}">
     <text>This includes 13 prospective studies from different regions; 0.42 estimate was Kenya-specific but they have Europe, France specifically, and other African countries</text>
   </threadedComment>
-  <threadedComment ref="M15" dT="2025-01-22T18:20:02.26" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
+  <threadedComment ref="N15" dT="2025-01-22T18:20:02.26" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
     <text>Update to WHO reference because this is actually a global estimate</text>
-  </threadedComment>
-  <threadedComment ref="G49" dT="2025-02-12T20:18:59.04" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{41F30597-8EA5-6B4E-BC92-48BBEE4F0910}">
-    <text>Consider using IeDEA data for Kenya as well and fit a similar model</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B2D996-732D-784F-96EB-809CE760E324}">
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R55" sqref="R55"/>
+      <selection pane="bottomRight" activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2301,17 +2302,17 @@
     <col min="6" max="6" width="55" style="5" customWidth="1"/>
     <col min="7" max="8" width="53.5" style="5" customWidth="1"/>
     <col min="9" max="9" width="53.5" style="5" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="53.5" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17" style="5" customWidth="1"/>
-    <col min="13" max="13" width="24" style="5" customWidth="1"/>
-    <col min="14" max="14" width="26" style="5" customWidth="1"/>
-    <col min="15" max="15" width="37.5" style="5" customWidth="1"/>
-    <col min="16" max="16" width="30.5" style="5" hidden="1" customWidth="1"/>
-    <col min="17" max="18" width="30.5" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="5"/>
+    <col min="10" max="12" width="53.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17" style="5" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="5" customWidth="1"/>
+    <col min="15" max="15" width="26" style="5" customWidth="1"/>
+    <col min="16" max="16" width="37.5" style="5" customWidth="1"/>
+    <col min="17" max="17" width="30.5" style="5" hidden="1" customWidth="1"/>
+    <col min="18" max="20" width="30.5" style="5" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -2335,19 +2336,21 @@
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="N1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="64"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="37"/>
       <c r="R1" s="64"/>
-    </row>
-    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+    </row>
+    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="38"/>
       <c r="B2" s="40"/>
       <c r="C2" s="42"/>
@@ -2366,32 +2369,38 @@
         <v>24</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="M2" s="39"/>
+      <c r="N2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="O2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="P2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="Q2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="64" t="s">
-        <v>196</v>
-      </c>
       <c r="R2" s="64" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="211" customHeight="1" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+      <c r="S2" s="64" t="s">
+        <v>198</v>
+      </c>
+      <c r="T2" s="64" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="211" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>33</v>
       </c>
@@ -2406,38 +2415,44 @@
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G3" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>172</v>
-      </c>
       <c r="J3" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="25"/>
+      <c r="P3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R3" s="25"/>
-    </row>
-    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+    </row>
+    <row r="4" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
@@ -2459,25 +2474,27 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="25"/>
+      <c r="P4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R4" s="25"/>
-    </row>
-    <row r="5" spans="1:18" ht="272" x14ac:dyDescent="0.2">
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+    </row>
+    <row r="5" spans="1:20" ht="272" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>148</v>
       </c>
@@ -2497,41 +2514,47 @@
         <v>156</v>
       </c>
       <c r="G5" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="H5" s="59" t="s">
-        <v>211</v>
-      </c>
       <c r="I5" s="59" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J5" s="59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K5" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="L5" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="M5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="20"/>
+      <c r="O5" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="O5" s="27" t="s">
+      <c r="P5" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="P5" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q5" s="59" t="s">
-        <v>213</v>
+      <c r="Q5" s="29" t="s">
+        <v>190</v>
       </c>
       <c r="R5" s="59" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="S5" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="T5" s="59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>150</v>
       </c>
@@ -2558,32 +2581,38 @@
         <v>152</v>
       </c>
       <c r="J6" s="59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K6" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="L6" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="M6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="20"/>
+      <c r="O6" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="27" t="s">
+      <c r="P6" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="P6" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q6" s="59" t="s">
-        <v>213</v>
+      <c r="Q6" s="29" t="s">
+        <v>190</v>
       </c>
       <c r="R6" s="59" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="S6" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="T6" s="59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>67</v>
       </c>
@@ -2607,25 +2636,27 @@
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="18"/>
+      <c r="M7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="25"/>
+      <c r="P7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R7" s="25"/>
-    </row>
-    <row r="8" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+    </row>
+    <row r="8" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>69</v>
       </c>
@@ -2649,25 +2680,27 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="18"/>
+      <c r="M8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="25"/>
+      <c r="P8" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R8" s="25"/>
-    </row>
-    <row r="9" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+    </row>
+    <row r="9" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>68</v>
       </c>
@@ -2691,25 +2724,27 @@
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="18"/>
+      <c r="M9" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O9" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="25"/>
+      <c r="P9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R9" s="25"/>
-    </row>
-    <row r="10" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+    </row>
+    <row r="10" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>70</v>
       </c>
@@ -2733,25 +2768,27 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="18"/>
+      <c r="M10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="25" t="s">
+      <c r="N10" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="25"/>
+      <c r="P10" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R10" s="25"/>
-    </row>
-    <row r="11" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+    </row>
+    <row r="11" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>6</v>
       </c>
@@ -2775,19 +2812,21 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="18"/>
+      <c r="M11" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="N11" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="N11" s="27"/>
       <c r="O11" s="27"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="25"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="29"/>
       <c r="R11" s="25"/>
-    </row>
-    <row r="12" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+    </row>
+    <row r="12" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>7</v>
       </c>
@@ -2801,19 +2840,19 @@
         <v>32</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>49</v>
       </c>
       <c r="G12" s="63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H12" s="27" t="s">
         <v>85</v>
       </c>
       <c r="I12" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J12" s="27" t="s">
         <v>85</v>
@@ -2821,27 +2860,33 @@
       <c r="K12" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="20"/>
-      <c r="N12" s="27" t="s">
-        <v>195</v>
-      </c>
+      <c r="N12" s="20"/>
       <c r="O12" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P12" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="Q12" s="25" t="s">
-        <v>195</v>
+      <c r="Q12" s="27" t="s">
+        <v>193</v>
       </c>
       <c r="R12" s="25" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+      <c r="S12" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="T12" s="25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>73</v>
       </c>
@@ -2865,25 +2910,27 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="18"/>
+      <c r="M13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="25" t="s">
+      <c r="N13" s="26" t="s">
         <v>2</v>
       </c>
       <c r="O13" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P13" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="25"/>
+      <c r="P13" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="R13" s="25"/>
-    </row>
-    <row r="14" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+    </row>
+    <row r="14" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>75</v>
       </c>
@@ -2913,25 +2960,31 @@
       <c r="K14" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="30" t="s">
+      <c r="L14" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="20"/>
-      <c r="N14" s="27" t="s">
-        <v>61</v>
-      </c>
+      <c r="N14" s="20"/>
       <c r="O14" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="25" t="s">
+      <c r="P14" s="27" t="s">
         <v>61</v>
       </c>
+      <c r="Q14" s="32"/>
       <c r="R14" s="25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="S14" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="T14" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>77</v>
       </c>
@@ -2955,21 +3008,23 @@
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="30" t="s">
+      <c r="L15" s="18"/>
+      <c r="M15" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="30" t="s">
+      <c r="N15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="N15" s="18" t="s">
+      <c r="O15" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="19"/>
       <c r="R15" s="18"/>
-    </row>
-    <row r="16" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+    </row>
+    <row r="16" spans="1:20" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>37</v>
       </c>
@@ -2983,7 +3038,7 @@
         <v>32</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>116</v>
@@ -2993,19 +3048,21 @@
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="18"/>
+      <c r="M16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="N16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="N16" s="18"/>
       <c r="O16" s="18"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="19"/>
       <c r="R16" s="18"/>
-    </row>
-    <row r="17" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+    </row>
+    <row r="17" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>117</v>
       </c>
@@ -3029,25 +3086,27 @@
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="18"/>
+      <c r="M17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N17" s="10" t="s">
+      <c r="N17" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="10"/>
+      <c r="P17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R17" s="10"/>
-    </row>
-    <row r="18" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>118</v>
       </c>
@@ -3071,25 +3130,27 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="18"/>
+      <c r="M18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P18" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q18" s="10"/>
+      <c r="P18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R18" s="10"/>
-    </row>
-    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>119</v>
       </c>
@@ -3113,25 +3174,27 @@
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="18"/>
+      <c r="M19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M19" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P19" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="10"/>
+      <c r="P19" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R19" s="10"/>
-    </row>
-    <row r="20" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>120</v>
       </c>
@@ -3155,25 +3218,27 @@
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="18"/>
+      <c r="M20" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P20" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="10"/>
+      <c r="P20" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R20" s="10"/>
-    </row>
-    <row r="21" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>121</v>
       </c>
@@ -3197,25 +3262,27 @@
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
-      <c r="L21" s="13" t="s">
+      <c r="L21" s="18"/>
+      <c r="M21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M21" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N21" s="10" t="s">
+      <c r="N21" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P21" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="10"/>
+      <c r="P21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R21" s="10"/>
-    </row>
-    <row r="22" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="22" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>122</v>
       </c>
@@ -3239,25 +3306,27 @@
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
-      <c r="L22" s="13" t="s">
+      <c r="L22" s="18"/>
+      <c r="M22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M22" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N22" s="10" t="s">
+      <c r="N22" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O22" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P22" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="10"/>
+      <c r="P22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R22" s="10"/>
-    </row>
-    <row r="23" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+    </row>
+    <row r="23" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>129</v>
       </c>
@@ -3281,25 +3350,27 @@
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="13" t="s">
+      <c r="L23" s="18"/>
+      <c r="M23" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M23" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N23" s="10" t="s">
+      <c r="N23" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="10"/>
+      <c r="P23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R23" s="10"/>
-    </row>
-    <row r="24" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>130</v>
       </c>
@@ -3323,25 +3394,27 @@
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="13" t="s">
+      <c r="L24" s="18"/>
+      <c r="M24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M24" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N24" s="10" t="s">
+      <c r="N24" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P24" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q24" s="10"/>
+      <c r="P24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R24" s="10"/>
-    </row>
-    <row r="25" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>131</v>
       </c>
@@ -3365,25 +3438,27 @@
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="18"/>
+      <c r="M25" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M25" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N25" s="10" t="s">
+      <c r="N25" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P25" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q25" s="10"/>
+      <c r="P25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R25" s="10"/>
-    </row>
-    <row r="26" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+    </row>
+    <row r="26" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>132</v>
       </c>
@@ -3407,25 +3482,27 @@
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="13" t="s">
+      <c r="L26" s="18"/>
+      <c r="M26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M26" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N26" s="10" t="s">
+      <c r="N26" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P26" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q26" s="10"/>
+      <c r="P26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R26" s="10"/>
-    </row>
-    <row r="27" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+    </row>
+    <row r="27" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>133</v>
       </c>
@@ -3449,25 +3526,27 @@
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
-      <c r="L27" s="13" t="s">
+      <c r="L27" s="18"/>
+      <c r="M27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M27" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N27" s="10" t="s">
+      <c r="N27" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P27" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q27" s="10"/>
+      <c r="P27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R27" s="10"/>
-    </row>
-    <row r="28" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>134</v>
       </c>
@@ -3491,25 +3570,27 @@
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
-      <c r="L28" s="13" t="s">
+      <c r="L28" s="18"/>
+      <c r="M28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N28" s="10" t="s">
+      <c r="N28" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P28" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q28" s="10"/>
+      <c r="P28" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="R28" s="10"/>
-    </row>
-    <row r="29" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+    </row>
+    <row r="29" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>89</v>
       </c>
@@ -3517,16 +3598,16 @@
         <v>38</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G29" s="14">
         <v>4.0579709999999998E-2</v>
@@ -3538,24 +3619,26 @@
         <v>5.3571430000000003E-2</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="L29" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="L29" s="14"/>
+      <c r="M29" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M29" s="16" t="s">
+      <c r="N29" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N29" s="14"/>
       <c r="O29" s="14"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="15"/>
       <c r="R29" s="14"/>
-    </row>
-    <row r="30" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+    </row>
+    <row r="30" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>14</v>
       </c>
@@ -3563,14 +3646,14 @@
         <v>38</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G30" s="14">
         <v>8.1250000000000003E-2</v>
@@ -3582,24 +3665,26 @@
         <v>2.272727E-3</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="L30" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="L30" s="14"/>
+      <c r="M30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M30" s="16" t="s">
+      <c r="N30" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N30" s="14"/>
       <c r="O30" s="14"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="15"/>
       <c r="R30" s="14"/>
-    </row>
-    <row r="31" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+    </row>
+    <row r="31" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>15</v>
       </c>
@@ -3607,14 +3692,14 @@
         <v>38</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G31" s="14">
         <v>0.02</v>
@@ -3626,24 +3711,26 @@
         <v>3.9473679999999997E-3</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="L31" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="L31" s="14"/>
+      <c r="M31" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="N31" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="14"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="15"/>
       <c r="R31" s="14"/>
-    </row>
-    <row r="32" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+    </row>
+    <row r="32" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>143</v>
       </c>
@@ -3665,25 +3752,27 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="16" t="s">
+      <c r="L32" s="18"/>
+      <c r="M32" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="N32" s="14" t="s">
+      <c r="N32" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O32" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P32" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q32" s="14"/>
+      <c r="P32" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="R32" s="14"/>
-    </row>
-    <row r="33" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+    </row>
+    <row r="33" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>147</v>
       </c>
@@ -3705,25 +3794,27 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="16" t="s">
+      <c r="L33" s="18"/>
+      <c r="M33" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="N33" s="14" t="s">
+      <c r="N33" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O33" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P33" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="14"/>
+      <c r="P33" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="R33" s="14"/>
-    </row>
-    <row r="34" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+    </row>
+    <row r="34" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>144</v>
       </c>
@@ -3745,25 +3836,27 @@
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="16" t="s">
+      <c r="L34" s="18"/>
+      <c r="M34" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M34" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="N34" s="14" t="s">
+      <c r="N34" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O34" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P34" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="14"/>
+      <c r="P34" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="R34" s="14"/>
-    </row>
-    <row r="35" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+    </row>
+    <row r="35" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>145</v>
       </c>
@@ -3785,25 +3878,27 @@
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="18"/>
-      <c r="L35" s="16" t="s">
+      <c r="L35" s="18"/>
+      <c r="M35" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M35" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="N35" s="14" t="s">
+      <c r="N35" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P35" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q35" s="14"/>
+      <c r="P35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="R35" s="14"/>
-    </row>
-    <row r="36" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+    </row>
+    <row r="36" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>146</v>
       </c>
@@ -3825,25 +3920,27 @@
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="16" t="s">
+      <c r="L36" s="18"/>
+      <c r="M36" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M36" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="N36" s="14" t="s">
+      <c r="N36" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O36" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P36" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q36" s="14"/>
+      <c r="P36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="R36" s="14"/>
-    </row>
-    <row r="37" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+    </row>
+    <row r="37" spans="1:20" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="44" t="s">
         <v>108</v>
       </c>
@@ -3865,19 +3962,21 @@
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="18"/>
-      <c r="L37" s="48" t="s">
+      <c r="L37" s="18"/>
+      <c r="M37" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="M37" s="51" t="s">
+      <c r="N37" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="N37" s="36"/>
       <c r="O37" s="36"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="36"/>
+      <c r="P37" s="36"/>
+      <c r="Q37" s="58"/>
       <c r="R37" s="36"/>
-    </row>
-    <row r="38" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S37" s="36"/>
+      <c r="T37" s="36"/>
+    </row>
+    <row r="38" spans="1:20" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
         <v>16</v>
       </c>
@@ -3901,25 +4000,27 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
-      <c r="L38" s="48" t="s">
+      <c r="L38" s="18"/>
+      <c r="M38" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M38" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="N38" s="52" t="s">
+      <c r="N38" s="51" t="s">
         <v>2</v>
       </c>
       <c r="O38" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="P38" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q38" s="52"/>
+      <c r="P38" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="53" t="s">
+        <v>2</v>
+      </c>
       <c r="R38" s="52"/>
-    </row>
-    <row r="39" spans="1:18" ht="170" x14ac:dyDescent="0.2">
+      <c r="S38" s="52"/>
+      <c r="T38" s="52"/>
+    </row>
+    <row r="39" spans="1:20" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="44" t="s">
         <v>90</v>
       </c>
@@ -3943,25 +4044,27 @@
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
-      <c r="L39" s="48" t="s">
+      <c r="L39" s="18"/>
+      <c r="M39" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="M39" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="N39" s="44" t="s">
+      <c r="N39" s="48" t="s">
         <v>17</v>
       </c>
       <c r="O39" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="P39" s="45" t="s">
+      <c r="P39" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="Q39" s="44"/>
+      <c r="Q39" s="45" t="s">
+        <v>17</v>
+      </c>
       <c r="R39" s="44"/>
-    </row>
-    <row r="40" spans="1:18" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+    </row>
+    <row r="40" spans="1:20" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44" t="s">
         <v>19</v>
       </c>
@@ -3989,25 +4092,27 @@
       <c r="I40" s="44"/>
       <c r="J40" s="44"/>
       <c r="K40" s="44"/>
-      <c r="L40" s="48" t="s">
+      <c r="L40" s="44"/>
+      <c r="M40" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M40" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="N40" s="55" t="s">
+      <c r="N40" s="54" t="s">
         <v>2</v>
       </c>
       <c r="O40" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="P40" s="56" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q40" s="55"/>
+      <c r="P40" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q40" s="56" t="s">
+        <v>2</v>
+      </c>
       <c r="R40" s="55"/>
-    </row>
-    <row r="41" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S40" s="55"/>
+      <c r="T40" s="55"/>
+    </row>
+    <row r="41" spans="1:20" ht="40" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="44" t="s">
         <v>21</v>
       </c>
@@ -4033,25 +4138,27 @@
       <c r="I41" s="44"/>
       <c r="J41" s="44"/>
       <c r="K41" s="44"/>
-      <c r="L41" s="48" t="s">
+      <c r="L41" s="44"/>
+      <c r="M41" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M41" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="N41" s="44" t="s">
+      <c r="N41" s="48" t="s">
         <v>2</v>
       </c>
       <c r="O41" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P41" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q41" s="44"/>
+      <c r="P41" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q41" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="R41" s="44"/>
-    </row>
-    <row r="42" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+    </row>
+    <row r="42" spans="1:20" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
         <v>40</v>
       </c>
@@ -4077,25 +4184,27 @@
       <c r="I42" s="44"/>
       <c r="J42" s="44"/>
       <c r="K42" s="44"/>
-      <c r="L42" s="48" t="s">
+      <c r="L42" s="44"/>
+      <c r="M42" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M42" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="N42" s="44" t="s">
+      <c r="N42" s="48" t="s">
         <v>2</v>
       </c>
       <c r="O42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P42" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q42" s="44"/>
+      <c r="P42" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="R42" s="44"/>
-    </row>
-    <row r="43" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S42" s="44"/>
+      <c r="T42" s="44"/>
+    </row>
+    <row r="43" spans="1:20" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="44" t="s">
         <v>41</v>
       </c>
@@ -4121,25 +4230,27 @@
       <c r="I43" s="44"/>
       <c r="J43" s="44"/>
       <c r="K43" s="44"/>
-      <c r="L43" s="48" t="s">
+      <c r="L43" s="44"/>
+      <c r="M43" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M43" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="N43" s="44" t="s">
+      <c r="N43" s="48" t="s">
         <v>2</v>
       </c>
       <c r="O43" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P43" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q43" s="44"/>
+      <c r="P43" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q43" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="R43" s="44"/>
-    </row>
-    <row r="44" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+    </row>
+    <row r="44" spans="1:20" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44" t="s">
         <v>42</v>
       </c>
@@ -4165,25 +4276,27 @@
       <c r="I44" s="44"/>
       <c r="J44" s="44"/>
       <c r="K44" s="44"/>
-      <c r="L44" s="48" t="s">
+      <c r="L44" s="44"/>
+      <c r="M44" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M44" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="N44" s="44" t="s">
+      <c r="N44" s="48" t="s">
         <v>2</v>
       </c>
       <c r="O44" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P44" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q44" s="44"/>
+      <c r="P44" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q44" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="R44" s="44"/>
-    </row>
-    <row r="45" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S44" s="44"/>
+      <c r="T44" s="44"/>
+    </row>
+    <row r="45" spans="1:20" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="44" t="s">
         <v>43</v>
       </c>
@@ -4204,30 +4317,32 @@
         <v>1</v>
       </c>
       <c r="H45" s="49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I45" s="44"/>
       <c r="J45" s="44"/>
       <c r="K45" s="44"/>
-      <c r="L45" s="48" t="s">
+      <c r="L45" s="44"/>
+      <c r="M45" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="M45" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="N45" s="44" t="s">
+      <c r="N45" s="48" t="s">
         <v>2</v>
       </c>
       <c r="O45" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P45" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q45" s="44"/>
+      <c r="P45" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q45" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="R45" s="44"/>
-    </row>
-    <row r="46" spans="1:18" ht="276" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S45" s="44"/>
+      <c r="T45" s="44"/>
+    </row>
+    <row r="46" spans="1:20" ht="276" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>78</v>
       </c>
@@ -4253,31 +4368,37 @@
         <v>163</v>
       </c>
       <c r="I46" s="31"/>
-      <c r="J46" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="K46" s="65" t="s">
-        <v>213</v>
-      </c>
-      <c r="L46" s="8" t="s">
+      <c r="J46" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M46" s="20"/>
-      <c r="N46" s="6" t="s">
+      <c r="N46" s="20"/>
+      <c r="O46" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="O46" s="6" t="s">
+      <c r="P46" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="6" t="s">
-        <v>213</v>
-      </c>
+      <c r="Q46" s="32"/>
       <c r="R46" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="S46" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="T46" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>98</v>
       </c>
@@ -4301,25 +4422,27 @@
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
-      <c r="L47" s="8" t="s">
+      <c r="L47" s="18"/>
+      <c r="M47" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M47" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N47" s="6" t="s">
+      <c r="N47" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O47" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P47" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q47" s="6"/>
+      <c r="P47" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R47" s="6"/>
-    </row>
-    <row r="48" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
+    </row>
+    <row r="48" spans="1:20" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>99</v>
       </c>
@@ -4343,25 +4466,27 @@
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
       <c r="K48" s="18"/>
-      <c r="L48" s="8" t="s">
+      <c r="L48" s="18"/>
+      <c r="M48" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M48" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N48" s="6" t="s">
+      <c r="N48" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O48" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P48" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q48" s="6"/>
+      <c r="P48" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q48" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R48" s="6"/>
-    </row>
-    <row r="49" spans="1:18" ht="227" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S48" s="6"/>
+      <c r="T48" s="6"/>
+    </row>
+    <row r="49" spans="1:20" ht="227" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>100</v>
       </c>
@@ -4378,40 +4503,46 @@
         <v>157</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G49" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="H49" s="60" t="s">
         <v>164</v>
-      </c>
-      <c r="H49" s="60" t="s">
-        <v>165</v>
       </c>
       <c r="I49" s="31"/>
       <c r="J49" s="65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K49" s="65" t="s">
-        <v>217</v>
-      </c>
-      <c r="L49" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="L49" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="M49" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M49" s="20"/>
-      <c r="N49" s="6" t="s">
+      <c r="N49" s="20"/>
+      <c r="O49" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O49" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="6" t="s">
-        <v>201</v>
-      </c>
+      <c r="P49" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q49" s="32"/>
       <c r="R49" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="S49" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="T49" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>159</v>
       </c>
@@ -4435,25 +4566,27 @@
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
-      <c r="L50" s="8" t="s">
+      <c r="L50" s="18"/>
+      <c r="M50" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M50" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N50" s="6" t="s">
+      <c r="N50" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O50" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P50" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q50" s="6"/>
+      <c r="P50" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R50" s="6"/>
-    </row>
-    <row r="51" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S50" s="6"/>
+      <c r="T50" s="6"/>
+    </row>
+    <row r="51" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
@@ -4461,7 +4594,7 @@
         <v>36</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>31</v>
@@ -4480,30 +4613,36 @@
       </c>
       <c r="I51" s="31"/>
       <c r="J51" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N51" s="20"/>
+      <c r="O51" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q51" s="32"/>
+      <c r="R51" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="K51" s="6" t="s">
+      <c r="S51" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="L51" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M51" s="20"/>
-      <c r="N51" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O51" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="R51" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T51" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
@@ -4511,7 +4650,7 @@
         <v>36</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>31</v>
@@ -4528,32 +4667,38 @@
       </c>
       <c r="I52" s="31"/>
       <c r="J52" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N52" s="20"/>
+      <c r="O52" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q52" s="32"/>
+      <c r="R52" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="K52" s="6" t="s">
+      <c r="S52" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="L52" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M52" s="20"/>
-      <c r="N52" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O52" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="P52" s="32"/>
-      <c r="Q52" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="R52" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="238" x14ac:dyDescent="0.2">
+      <c r="T52" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="238" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>36</v>
@@ -4565,43 +4710,49 @@
         <v>32</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G53" s="60" t="s">
+        <v>177</v>
+      </c>
+      <c r="H53" s="60" t="s">
+        <v>177</v>
+      </c>
+      <c r="I53" s="31"/>
+      <c r="J53" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="M53" s="8"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="T53" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="119" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="H53" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="I53" s="31"/>
-      <c r="J53" s="65" t="s">
-        <v>206</v>
-      </c>
-      <c r="K53" s="65" t="s">
-        <v>214</v>
-      </c>
-      <c r="L53" s="8"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="O53" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="P53" s="32"/>
-      <c r="Q53" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="R53" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="119" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>36</v>
@@ -4613,7 +4764,7 @@
         <v>31</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>161</v>
@@ -4621,27 +4772,29 @@
       <c r="G54" s="18"/>
       <c r="H54" s="57"/>
       <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="8" t="s">
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M54" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N54" s="6" t="s">
+      <c r="N54" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O54" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P54" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q54" s="6"/>
+      <c r="P54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q54" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R54" s="6"/>
-    </row>
-    <row r="55" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+    </row>
+    <row r="55" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>10</v>
       </c>
@@ -4649,7 +4802,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>31</v>
@@ -4665,29 +4818,37 @@
         <v>7.5484389999999998E-2</v>
       </c>
       <c r="I55" s="31"/>
-      <c r="J55" s="65" t="s">
-        <v>208</v>
-      </c>
-      <c r="K55" s="65"/>
-      <c r="L55" s="8" t="s">
+      <c r="J55" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M55" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="20"/>
-      <c r="N55" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="N55" s="20"/>
       <c r="O55" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="P55" s="32"/>
-      <c r="Q55" s="6" t="s">
-        <v>209</v>
-      </c>
+      <c r="P55" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q55" s="32"/>
       <c r="R55" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="S55" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>11</v>
       </c>
@@ -4709,25 +4870,27 @@
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
-      <c r="L56" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="M56" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N56" s="6" t="s">
+      <c r="L56" s="18"/>
+      <c r="M56" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="N56" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O56" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P56" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q56" s="6"/>
+      <c r="P56" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R56" s="6"/>
-    </row>
-    <row r="57" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+    </row>
+    <row r="57" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>12</v>
       </c>
@@ -4749,25 +4912,27 @@
       <c r="I57" s="18"/>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
-      <c r="L57" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="M57" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N57" s="6" t="s">
+      <c r="L57" s="18"/>
+      <c r="M57" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="N57" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P57" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q57" s="6"/>
+      <c r="P57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R57" s="6"/>
-    </row>
-    <row r="58" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+    </row>
+    <row r="58" spans="1:20" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>13</v>
       </c>
@@ -4789,25 +4954,27 @@
       <c r="I58" s="18"/>
       <c r="J58" s="18"/>
       <c r="K58" s="18"/>
-      <c r="L58" s="62" t="s">
-        <v>189</v>
-      </c>
-      <c r="M58" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="N58" s="6" t="s">
+      <c r="L58" s="18"/>
+      <c r="M58" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="N58" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O58" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P58" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q58" s="6"/>
+      <c r="P58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q58" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="R58" s="6"/>
-    </row>
-    <row r="59" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+    </row>
+    <row r="59" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>84</v>
       </c>
@@ -4835,9 +5002,6 @@
       <c r="I59" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="L59" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="M59" s="5" t="s">
         <v>84</v>
       </c>
@@ -4848,6 +5012,9 @@
         <v>84</v>
       </c>
       <c r="P59" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q59" s="5" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated France priors, added back to data manager, decoupled trates and allowed times to be sampled
</commit_message>
<xml_diff>
--- a/documentation/PARAMS.xlsx
+++ b/documentation/PARAMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287D7D8A-11E1-8C43-AC30-7B9C05210607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A456B-8B84-7B4F-B945-D0C0639631B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="272">
   <si>
     <t>Parameter</t>
   </si>
@@ -1928,6 +1928,64 @@
   </si>
   <si>
     <t>Ethiopia, DRC, CI, Ghana DHS surveys</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.141 - European estimate from Dabis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Logitnormal
+Begins at this value in 1990, interpolates to birth.transmission.risk.1 from 1990-2020</t>
+    </r>
+  </si>
+  <si>
+    <t>Bruyand et al, 2019
+Sicsic et al, 2016</t>
+  </si>
+  <si>
+    <t>Bruyand, 2019 and Sicsic, 2016 
+Bruyand: 2016 values by age*sex 
+Ages: 18-24, 25-39, 40-54, 55-75
+Sicsic, 2006-2013 values by total, age, and sex 
+Ages: 15-29,30-44,45-70
+Means are pretty low (~12%)</t>
+  </si>
+  <si>
+    <t>Cuzin, 2023</t>
+  </si>
+  <si>
+    <t>Cuzin, 2023: Dat'AIDS cohort, 2009-2019
+Median time from HIV diagnosis to ART prescription 128 days [33; 570] in 2009–2011 --&gt; annual proportion = 0.8951337 (after multiplied by max proportion)</t>
+  </si>
+  <si>
+    <t>0.0965109
+Estimate from Belgium</t>
+  </si>
+  <si>
+    <t>Belgium (Beckhoven, et al, 2015): https://link.springer.com/article/10.1186/s12879-015-1230-3</t>
+  </si>
+  <si>
+    <t>Cuzin, 2023: Dat'AIDS cohort, 2009-2019
+Median time from ART prescription to controlled VL 83 days --&gt; annual proportion = 0.9383084 (after multiplied by max proportion)</t>
+  </si>
+  <si>
+    <t>Cuzin et al, 2023
+Among those followed, 91% still had a controlled VL 1 year later --&gt; rate = 0.09431068</t>
   </si>
 </sst>
 </file>
@@ -2777,10 +2835,10 @@
   <dimension ref="A1:AF59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q46" sqref="Q46"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2791,15 +2849,12 @@
     <col min="4" max="4" width="10.6640625" style="5" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="5" customWidth="1"/>
     <col min="6" max="6" width="55" style="5" customWidth="1"/>
-    <col min="7" max="8" width="53.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="53.5" style="5" hidden="1" customWidth="1"/>
-    <col min="10" max="18" width="53.5" style="5" customWidth="1"/>
+    <col min="7" max="18" width="53.5" style="5" customWidth="1"/>
     <col min="19" max="19" width="17" style="5" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="24" style="5" customWidth="1"/>
     <col min="21" max="21" width="26" style="5" customWidth="1"/>
     <col min="22" max="22" width="37.5" style="5" customWidth="1"/>
-    <col min="23" max="23" width="30.5" style="5" hidden="1" customWidth="1"/>
-    <col min="24" max="32" width="30.5" style="5" customWidth="1"/>
+    <col min="23" max="32" width="30.5" style="5" customWidth="1"/>
     <col min="33" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
@@ -3708,7 +3763,9 @@
       <c r="H14" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="55" t="s">
+        <v>263</v>
+      </c>
       <c r="J14" s="27" t="s">
         <v>51</v>
       </c>
@@ -5530,7 +5587,9 @@
       <c r="H46" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="I46" s="31"/>
+      <c r="I46" s="56" t="s">
+        <v>265</v>
+      </c>
       <c r="J46" s="6" t="s">
         <v>191</v>
       </c>
@@ -5568,7 +5627,9 @@
       <c r="V46" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="W46" s="32"/>
+      <c r="W46" s="6" t="s">
+        <v>264</v>
+      </c>
       <c r="X46" s="6" t="s">
         <v>206</v>
       </c>
@@ -5732,7 +5793,9 @@
       <c r="H49" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="I49" s="31"/>
+      <c r="I49" s="56" t="s">
+        <v>267</v>
+      </c>
       <c r="J49" s="61" t="s">
         <v>196</v>
       </c>
@@ -5770,7 +5833,9 @@
       <c r="V49" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="W49" s="32"/>
+      <c r="W49" s="6" t="s">
+        <v>266</v>
+      </c>
       <c r="X49" s="6" t="s">
         <v>195</v>
       </c>
@@ -5878,7 +5943,9 @@
       <c r="H51" s="6">
         <v>0.15548490000000001</v>
       </c>
-      <c r="I51" s="31"/>
+      <c r="I51" s="6" t="s">
+        <v>268</v>
+      </c>
       <c r="J51" s="6" t="s">
         <v>198</v>
       </c>
@@ -5916,7 +5983,9 @@
       <c r="V51" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="W51" s="32"/>
+      <c r="W51" s="6" t="s">
+        <v>269</v>
+      </c>
       <c r="X51" s="6" t="s">
         <v>199</v>
       </c>
@@ -5968,7 +6037,9 @@
       <c r="H52" s="6">
         <v>0.15548490000000001</v>
       </c>
-      <c r="I52" s="31"/>
+      <c r="I52" s="6" t="s">
+        <v>268</v>
+      </c>
       <c r="J52" s="6" t="s">
         <v>198</v>
       </c>
@@ -6006,7 +6077,9 @@
       <c r="V52" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="W52" s="32"/>
+      <c r="W52" s="6" t="s">
+        <v>269</v>
+      </c>
       <c r="X52" s="6" t="s">
         <v>199</v>
       </c>
@@ -6056,7 +6129,9 @@
       <c r="H53" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="I53" s="31"/>
+      <c r="I53" s="56" t="s">
+        <v>270</v>
+      </c>
       <c r="J53" s="6" t="s">
         <v>220</v>
       </c>
@@ -6092,7 +6167,9 @@
       <c r="V53" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W53" s="32"/>
+      <c r="W53" s="6" t="s">
+        <v>266</v>
+      </c>
       <c r="X53" s="6" t="s">
         <v>200</v>
       </c>
@@ -6200,7 +6277,9 @@
       <c r="H55" s="6">
         <v>7.5484389999999998E-2</v>
       </c>
-      <c r="I55" s="31"/>
+      <c r="I55" s="6" t="s">
+        <v>271</v>
+      </c>
       <c r="J55" s="6" t="s">
         <v>201</v>
       </c>
@@ -6238,7 +6317,9 @@
       <c r="V55" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="W55" s="32"/>
+      <c r="W55" s="6" t="s">
+        <v>266</v>
+      </c>
       <c r="X55" s="6" t="s">
         <v>202</v>
       </c>

</xml_diff>

<commit_message>
getting thailand set up
</commit_message>
<xml_diff>
--- a/documentation/PARAMS.xlsx
+++ b/documentation/PARAMS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0218F3D-506D-A34B-ADED-9DECDD2D4572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC87050-615E-E743-A5BD-F42D6B94BCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22000" windowHeight="19560" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$W$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$X$59</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +45,7 @@
     <author>tc={51F972CD-9F3E-FF43-98B5-159579D7B474}</author>
   </authors>
   <commentList>
-    <comment ref="U14" authorId="0" shapeId="0" xr:uid="{04385ABF-366F-F14D-B686-003B7FD6A102}">
+    <comment ref="V14" authorId="0" shapeId="0" xr:uid="{04385ABF-366F-F14D-B686-003B7FD6A102}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -53,7 +53,7 @@
     This includes 13 prospective studies from different regions; 0.42 estimate was Kenya-specific but they have Europe, France specifically, and other African countries</t>
       </text>
     </comment>
-    <comment ref="T15" authorId="1" shapeId="0" xr:uid="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
+    <comment ref="U15" authorId="1" shapeId="0" xr:uid="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="279">
   <si>
     <t>Parameter</t>
   </si>
@@ -1986,6 +1986,43 @@
   <si>
     <t>Cuzin et al, 2023
 Among those followed, 91% still had a controlled VL 1 year later --&gt; rate = 0.09431068</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Hong Kong study (Smith 2023)</t>
+  </si>
+  <si>
+    <t>Smith et al, 2023</t>
+  </si>
+  <si>
+    <t>0.242
+1999 Bangkok hospital study 
+Logitnormal
+Begins at this value in 1990, interpolates to birth.transmission.risk.1 from 1990-2020</t>
+  </si>
+  <si>
+    <t>Mock et al, 1999</t>
+  </si>
+  <si>
+    <t>Years
+- 2006: National Sexual Behavior Survey
+- 2012: General population survey in urban region
+- 2014: General population survey in Chiang Mai 
+Age groups
+- 2006: 18-39, 40-49, 50-59; reference age = 40-49
+- 2012:  15-19, 20-24, 35-44, 45-54, 55-59; ref = 35-44
+- 2014: 15-19, 20-29, 30-39, 40-49, 50-59, 60+; ref = 30-39
+Calculation: 
+- 2006: (proportion having sex with a casual partner)*(1-condom use with a casual partner)
+- 2012: proportion having casual sex in the past 12 months (didn't report condom use)
+- 2014: proportion with &gt;1 sexual partner in past 3 months*(1-condom use in past 3 months)</t>
+  </si>
+  <si>
+    <t>Ford et al, 2009 (NSBS 2006)
+Techasrivichien et al, 2014
+Pinyopornpanish et al, 2017</t>
   </si>
 </sst>
 </file>
@@ -2821,10 +2858,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U14" dT="2025-01-22T18:42:38.64" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{04385ABF-366F-F14D-B686-003B7FD6A102}">
+  <threadedComment ref="V14" dT="2025-01-22T18:42:38.64" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{04385ABF-366F-F14D-B686-003B7FD6A102}">
     <text>This includes 13 prospective studies from different regions; 0.42 estimate was Kenya-specific but they have Europe, France specifically, and other African countries</text>
   </threadedComment>
-  <threadedComment ref="T15" dT="2025-01-22T18:20:02.26" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
+  <threadedComment ref="U15" dT="2025-01-22T18:20:02.26" personId="{FA2A8BF6-F7F9-E248-9793-CD9889996086}" id="{51F972CD-9F3E-FF43-98B5-159579D7B474}">
     <text>Update to WHO reference because this is actually a global estimate</text>
   </threadedComment>
 </ThreadedComments>
@@ -2832,13 +2869,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B2D996-732D-784F-96EB-809CE760E324}">
-  <dimension ref="A1:AF59"/>
+  <dimension ref="A1:AH59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W53" sqref="W53"/>
+      <selection pane="bottomRight" activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2849,16 +2886,16 @@
     <col min="4" max="4" width="10.6640625" style="5" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="5" customWidth="1"/>
     <col min="6" max="6" width="55" style="5" customWidth="1"/>
-    <col min="7" max="18" width="53.5" style="5" customWidth="1"/>
-    <col min="19" max="19" width="17" style="5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="24" style="5" customWidth="1"/>
-    <col min="21" max="21" width="26" style="5" customWidth="1"/>
-    <col min="22" max="22" width="37.5" style="5" customWidth="1"/>
-    <col min="23" max="32" width="30.5" style="5" customWidth="1"/>
-    <col min="33" max="16384" width="10.83203125" style="5"/>
+    <col min="7" max="19" width="53.5" style="5" customWidth="1"/>
+    <col min="20" max="20" width="17" style="5" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="24" style="5" customWidth="1"/>
+    <col min="22" max="22" width="26" style="5" customWidth="1"/>
+    <col min="23" max="23" width="37.5" style="5" customWidth="1"/>
+    <col min="24" max="34" width="30.5" style="5" customWidth="1"/>
+    <col min="35" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -2889,16 +2926,16 @@
       <c r="P1" s="69"/>
       <c r="Q1" s="69"/>
       <c r="R1" s="69"/>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="69"/>
+      <c r="T1" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="66" t="s">
+      <c r="U1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="35"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="60"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="36"/>
       <c r="Y1" s="60"/>
       <c r="Z1" s="60"/>
       <c r="AA1" s="60"/>
@@ -2907,8 +2944,10 @@
       <c r="AD1" s="60"/>
       <c r="AE1" s="60"/>
       <c r="AF1" s="60"/>
+      <c r="AG1" s="60"/>
+      <c r="AH1" s="60"/>
     </row>
-    <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" ht="60" x14ac:dyDescent="0.35">
       <c r="A2" s="37"/>
       <c r="B2" s="38"/>
       <c r="C2" s="39"/>
@@ -2948,53 +2987,59 @@
         <v>230</v>
       </c>
       <c r="Q2" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="R2" s="63" t="s">
         <v>236</v>
       </c>
-      <c r="R2" s="63" t="s">
+      <c r="S2" s="63" t="s">
         <v>237</v>
       </c>
-      <c r="S2" s="63"/>
-      <c r="T2" s="62" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="63" t="s">
+      <c r="V2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="63" t="s">
+      <c r="W2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="64" t="s">
+      <c r="X2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="65" t="s">
+      <c r="Y2" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="Y2" s="65" t="s">
+      <c r="Z2" s="65" t="s">
         <v>193</v>
       </c>
-      <c r="Z2" s="65" t="s">
+      <c r="AA2" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="AA2" s="65" t="s">
+      <c r="AB2" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="AB2" s="65" t="s">
+      <c r="AC2" s="65" t="s">
         <v>218</v>
       </c>
-      <c r="AC2" s="65" t="s">
+      <c r="AD2" s="65" t="s">
         <v>227</v>
       </c>
-      <c r="AD2" s="65" t="s">
+      <c r="AE2" s="65" t="s">
         <v>230</v>
       </c>
-      <c r="AE2" s="63" t="s">
+      <c r="AF2" s="65" t="s">
+        <v>272</v>
+      </c>
+      <c r="AG2" s="63" t="s">
         <v>236</v>
       </c>
-      <c r="AF2" s="63" t="s">
+      <c r="AH2" s="63" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="211" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="211" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>33</v>
       </c>
@@ -3042,25 +3087,27 @@
         <v>235</v>
       </c>
       <c r="Q3" s="25" t="s">
-        <v>238</v>
+        <v>192</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U3" s="25" t="s">
+      <c r="S3" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X3" s="25"/>
+      <c r="W3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y3" s="25"/>
       <c r="Z3" s="25"/>
       <c r="AA3" s="25"/>
@@ -3069,8 +3116,10 @@
       <c r="AD3" s="25"/>
       <c r="AE3" s="25"/>
       <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
     </row>
-    <row r="4" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
@@ -3099,22 +3148,22 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
-      <c r="S4" s="30" t="s">
+      <c r="S4" s="18"/>
+      <c r="T4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U4" s="25" t="s">
+      <c r="U4" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W4" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X4" s="25"/>
+      <c r="W4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y4" s="25"/>
       <c r="Z4" s="25"/>
       <c r="AA4" s="25"/>
@@ -3123,8 +3172,10 @@
       <c r="AD4" s="25"/>
       <c r="AE4" s="25"/>
       <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
     </row>
-    <row r="5" spans="1:32" ht="272" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" ht="306" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>147</v>
       </c>
@@ -3174,53 +3225,59 @@
         <v>231</v>
       </c>
       <c r="Q5" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="R5" s="55" t="s">
         <v>261</v>
       </c>
-      <c r="R5" s="55" t="s">
+      <c r="S5" s="55" t="s">
         <v>251</v>
       </c>
-      <c r="S5" s="30" t="s">
+      <c r="T5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="20"/>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="20"/>
+      <c r="V5" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="W5" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="W5" s="29" t="s">
+      <c r="X5" s="29" t="s">
         <v>185</v>
-      </c>
-      <c r="X5" s="55" t="s">
-        <v>206</v>
       </c>
       <c r="Y5" s="55" t="s">
         <v>206</v>
       </c>
       <c r="Z5" s="55" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA5" s="55" t="s">
         <v>215</v>
       </c>
-      <c r="AA5" s="55" t="s">
+      <c r="AB5" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="AB5" s="55" t="s">
+      <c r="AC5" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="AC5" s="55" t="s">
+      <c r="AD5" s="55" t="s">
         <v>228</v>
       </c>
-      <c r="AD5" s="55" t="s">
+      <c r="AE5" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="AE5" s="55" t="s">
+      <c r="AF5" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="AG5" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="AF5" s="55" t="s">
+      <c r="AH5" s="55" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>149</v>
       </c>
@@ -3273,21 +3330,21 @@
       <c r="R6" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="S6" s="30" t="s">
+      <c r="S6" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="T6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="20"/>
-      <c r="U6" s="27" t="s">
+      <c r="U6" s="20"/>
+      <c r="V6" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="27" t="s">
+      <c r="W6" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="W6" s="29" t="s">
+      <c r="X6" s="29" t="s">
         <v>185</v>
-      </c>
-      <c r="X6" s="55" t="s">
-        <v>226</v>
       </c>
       <c r="Y6" s="55" t="s">
         <v>226</v>
@@ -3313,8 +3370,14 @@
       <c r="AF6" s="55" t="s">
         <v>226</v>
       </c>
+      <c r="AG6" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH6" s="55" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>67</v>
       </c>
@@ -3345,22 +3408,22 @@
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
-      <c r="S7" s="30" t="s">
+      <c r="S7" s="18"/>
+      <c r="T7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T7" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U7" s="25" t="s">
+      <c r="U7" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W7" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X7" s="25"/>
+      <c r="W7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y7" s="25"/>
       <c r="Z7" s="25"/>
       <c r="AA7" s="25"/>
@@ -3369,8 +3432,10 @@
       <c r="AD7" s="25"/>
       <c r="AE7" s="25"/>
       <c r="AF7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
     </row>
-    <row r="8" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>69</v>
       </c>
@@ -3401,22 +3466,22 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
-      <c r="S8" s="30" t="s">
+      <c r="S8" s="18"/>
+      <c r="T8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T8" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U8" s="25" t="s">
+      <c r="U8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W8" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X8" s="25"/>
+      <c r="W8" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y8" s="25"/>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25"/>
@@ -3425,8 +3490,10 @@
       <c r="AD8" s="25"/>
       <c r="AE8" s="25"/>
       <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
     </row>
-    <row r="9" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>68</v>
       </c>
@@ -3457,22 +3524,22 @@
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
-      <c r="S9" s="30" t="s">
+      <c r="S9" s="18"/>
+      <c r="T9" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T9" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U9" s="25" t="s">
+      <c r="U9" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V9" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W9" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X9" s="25"/>
+      <c r="W9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y9" s="25"/>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25"/>
@@ -3481,8 +3548,10 @@
       <c r="AD9" s="25"/>
       <c r="AE9" s="25"/>
       <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
     </row>
-    <row r="10" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>70</v>
       </c>
@@ -3513,22 +3582,22 @@
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
-      <c r="S10" s="30" t="s">
+      <c r="S10" s="18"/>
+      <c r="T10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T10" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U10" s="25" t="s">
+      <c r="U10" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W10" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X10" s="25"/>
+      <c r="W10" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y10" s="25"/>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25"/>
@@ -3537,8 +3606,10 @@
       <c r="AD10" s="25"/>
       <c r="AE10" s="25"/>
       <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
     </row>
-    <row r="11" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>6</v>
       </c>
@@ -3569,16 +3640,16 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
-      <c r="S11" s="30" t="s">
+      <c r="S11" s="18"/>
+      <c r="T11" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="T11" s="30" t="s">
+      <c r="U11" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="U11" s="27"/>
       <c r="V11" s="27"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="25"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="29"/>
       <c r="Y11" s="25"/>
       <c r="Z11" s="25"/>
       <c r="AA11" s="25"/>
@@ -3587,8 +3658,10 @@
       <c r="AD11" s="25"/>
       <c r="AE11" s="25"/>
       <c r="AF11" s="25"/>
+      <c r="AG11" s="25"/>
+      <c r="AH11" s="25"/>
     </row>
-    <row r="12" spans="1:32" ht="136" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>7</v>
       </c>
@@ -3637,27 +3710,27 @@
       <c r="P12" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" s="71" t="s">
+      <c r="Q12" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="R12" s="71" t="s">
         <v>257</v>
       </c>
-      <c r="R12" s="71" t="s">
+      <c r="S12" s="71" t="s">
         <v>258</v>
       </c>
-      <c r="S12" s="30" t="s">
+      <c r="T12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="T12" s="20"/>
-      <c r="U12" s="27" t="s">
-        <v>189</v>
-      </c>
+      <c r="U12" s="20"/>
       <c r="V12" s="27" t="s">
         <v>189</v>
       </c>
       <c r="W12" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="X12" s="27" t="s">
         <v>188</v>
-      </c>
-      <c r="X12" s="25" t="s">
-        <v>189</v>
       </c>
       <c r="Y12" s="25" t="s">
         <v>189</v>
@@ -3681,10 +3754,16 @@
         <v>189</v>
       </c>
       <c r="AF12" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="AG12" s="25" t="s">
         <v>189</v>
       </c>
+      <c r="AH12" s="25" t="s">
+        <v>189</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>73</v>
       </c>
@@ -3713,24 +3792,24 @@
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
       <c r="P13" s="18"/>
-      <c r="Q13" s="31"/>
+      <c r="Q13" s="18"/>
       <c r="R13" s="31"/>
-      <c r="S13" s="30" t="s">
+      <c r="S13" s="31"/>
+      <c r="T13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="T13" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U13" s="25" t="s">
+      <c r="U13" s="26" t="s">
         <v>2</v>
       </c>
       <c r="V13" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="W13" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="X13" s="25"/>
+      <c r="W13" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="Y13" s="25"/>
       <c r="Z13" s="25"/>
       <c r="AA13" s="25"/>
@@ -3739,8 +3818,10 @@
       <c r="AD13" s="25"/>
       <c r="AE13" s="25"/>
       <c r="AF13" s="25"/>
+      <c r="AG13" s="25"/>
+      <c r="AH13" s="25"/>
     </row>
-    <row r="14" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>75</v>
       </c>
@@ -3787,24 +3868,26 @@
       <c r="P14" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" s="71" t="s">
+      <c r="Q14" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="R14" s="71" t="s">
         <v>259</v>
       </c>
-      <c r="R14" s="71" t="s">
+      <c r="S14" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="S14" s="30" t="s">
+      <c r="T14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="T14" s="20"/>
-      <c r="U14" s="27" t="s">
-        <v>61</v>
-      </c>
+      <c r="U14" s="20"/>
       <c r="V14" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="W14" s="32"/>
-      <c r="X14" s="25" t="s">
+      <c r="W14" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" s="27" t="s">
         <v>61</v>
       </c>
       <c r="Y14" s="25" t="s">
@@ -3829,10 +3912,16 @@
         <v>61</v>
       </c>
       <c r="AF14" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG14" s="25" t="s">
         <v>61</v>
       </c>
+      <c r="AH14" s="25" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" ht="102" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>77</v>
       </c>
@@ -3863,18 +3952,18 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
-      <c r="S15" s="30" t="s">
+      <c r="S15" s="18"/>
+      <c r="T15" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="T15" s="30" t="s">
+      <c r="U15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="U15" s="18" t="s">
+      <c r="V15" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="V15" s="18"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="19"/>
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
@@ -3883,8 +3972,10 @@
       <c r="AD15" s="18"/>
       <c r="AE15" s="18"/>
       <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
     </row>
-    <row r="16" spans="1:32" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>37</v>
       </c>
@@ -3915,16 +4006,16 @@
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
-      <c r="S16" s="13" t="s">
+      <c r="S16" s="18"/>
+      <c r="T16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="U16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="U16" s="18"/>
       <c r="V16" s="18"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="19"/>
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
@@ -3933,8 +4024,10 @@
       <c r="AD16" s="18"/>
       <c r="AE16" s="18"/>
       <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="18"/>
     </row>
-    <row r="17" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>116</v>
       </c>
@@ -3965,22 +4058,22 @@
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
-      <c r="S17" s="13" t="s">
+      <c r="S17" s="18"/>
+      <c r="T17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T17" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U17" s="10" t="s">
+      <c r="U17" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X17" s="10"/>
+      <c r="W17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X17" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
@@ -3989,8 +4082,10 @@
       <c r="AD17" s="10"/>
       <c r="AE17" s="10"/>
       <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
     </row>
-    <row r="18" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>117</v>
       </c>
@@ -4021,22 +4116,22 @@
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
-      <c r="S18" s="13" t="s">
+      <c r="S18" s="18"/>
+      <c r="T18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T18" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U18" s="10" t="s">
+      <c r="U18" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W18" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X18" s="10"/>
+      <c r="W18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X18" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="10"/>
       <c r="AA18" s="10"/>
@@ -4045,8 +4140,10 @@
       <c r="AD18" s="10"/>
       <c r="AE18" s="10"/>
       <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
     </row>
-    <row r="19" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>118</v>
       </c>
@@ -4077,22 +4174,22 @@
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="18"/>
-      <c r="S19" s="13" t="s">
+      <c r="S19" s="18"/>
+      <c r="T19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T19" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U19" s="10" t="s">
+      <c r="U19" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W19" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X19" s="10"/>
+      <c r="W19" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
       <c r="AA19" s="10"/>
@@ -4101,8 +4198,10 @@
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
       <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
     </row>
-    <row r="20" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>119</v>
       </c>
@@ -4133,22 +4232,22 @@
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="18"/>
-      <c r="S20" s="13" t="s">
+      <c r="S20" s="18"/>
+      <c r="T20" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T20" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U20" s="10" t="s">
+      <c r="U20" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W20" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X20" s="10"/>
+      <c r="W20" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X20" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y20" s="10"/>
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
@@ -4157,8 +4256,10 @@
       <c r="AD20" s="10"/>
       <c r="AE20" s="10"/>
       <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
     </row>
-    <row r="21" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>120</v>
       </c>
@@ -4189,22 +4290,22 @@
       <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
-      <c r="S21" s="13" t="s">
+      <c r="S21" s="18"/>
+      <c r="T21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T21" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U21" s="10" t="s">
+      <c r="U21" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W21" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X21" s="10"/>
+      <c r="W21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="10"/>
@@ -4213,8 +4314,10 @@
       <c r="AD21" s="10"/>
       <c r="AE21" s="10"/>
       <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
     </row>
-    <row r="22" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>121</v>
       </c>
@@ -4245,22 +4348,22 @@
       <c r="P22" s="18"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="18"/>
-      <c r="S22" s="13" t="s">
+      <c r="S22" s="18"/>
+      <c r="T22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T22" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U22" s="10" t="s">
+      <c r="U22" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V22" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W22" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X22" s="10"/>
+      <c r="W22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X22" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y22" s="10"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="10"/>
@@ -4269,8 +4372,10 @@
       <c r="AD22" s="10"/>
       <c r="AE22" s="10"/>
       <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
     </row>
-    <row r="23" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>128</v>
       </c>
@@ -4301,22 +4406,22 @@
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="18"/>
-      <c r="S23" s="13" t="s">
+      <c r="S23" s="18"/>
+      <c r="T23" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T23" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U23" s="10" t="s">
+      <c r="U23" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W23" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X23" s="10"/>
+      <c r="W23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X23" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="10"/>
@@ -4325,8 +4430,10 @@
       <c r="AD23" s="10"/>
       <c r="AE23" s="10"/>
       <c r="AF23" s="10"/>
+      <c r="AG23" s="10"/>
+      <c r="AH23" s="10"/>
     </row>
-    <row r="24" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>129</v>
       </c>
@@ -4357,22 +4464,22 @@
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="18"/>
-      <c r="S24" s="13" t="s">
+      <c r="S24" s="18"/>
+      <c r="T24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T24" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U24" s="10" t="s">
+      <c r="U24" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W24" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X24" s="10"/>
+      <c r="W24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X24" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
@@ -4381,8 +4488,10 @@
       <c r="AD24" s="10"/>
       <c r="AE24" s="10"/>
       <c r="AF24" s="10"/>
+      <c r="AG24" s="10"/>
+      <c r="AH24" s="10"/>
     </row>
-    <row r="25" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>130</v>
       </c>
@@ -4413,22 +4522,22 @@
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
-      <c r="S25" s="13" t="s">
+      <c r="S25" s="18"/>
+      <c r="T25" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T25" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U25" s="10" t="s">
+      <c r="U25" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W25" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X25" s="10"/>
+      <c r="W25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X25" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
       <c r="AA25" s="10"/>
@@ -4437,8 +4546,10 @@
       <c r="AD25" s="10"/>
       <c r="AE25" s="10"/>
       <c r="AF25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="10"/>
     </row>
-    <row r="26" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>131</v>
       </c>
@@ -4469,22 +4580,22 @@
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
-      <c r="S26" s="13" t="s">
+      <c r="S26" s="18"/>
+      <c r="T26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T26" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U26" s="10" t="s">
+      <c r="U26" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W26" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X26" s="10"/>
+      <c r="W26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
       <c r="AA26" s="10"/>
@@ -4493,8 +4604,10 @@
       <c r="AD26" s="10"/>
       <c r="AE26" s="10"/>
       <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="10"/>
     </row>
-    <row r="27" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>132</v>
       </c>
@@ -4525,22 +4638,22 @@
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
-      <c r="S27" s="13" t="s">
+      <c r="S27" s="18"/>
+      <c r="T27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T27" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U27" s="10" t="s">
+      <c r="U27" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W27" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X27" s="10"/>
+      <c r="W27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X27" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y27" s="10"/>
       <c r="Z27" s="10"/>
       <c r="AA27" s="10"/>
@@ -4549,8 +4662,10 @@
       <c r="AD27" s="10"/>
       <c r="AE27" s="10"/>
       <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
     </row>
-    <row r="28" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>133</v>
       </c>
@@ -4581,22 +4696,22 @@
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="18"/>
-      <c r="S28" s="13" t="s">
+      <c r="S28" s="18"/>
+      <c r="T28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T28" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="U28" s="10" t="s">
+      <c r="U28" s="13" t="s">
         <v>2</v>
       </c>
       <c r="V28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W28" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="X28" s="10"/>
+      <c r="W28" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X28" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="Y28" s="10"/>
       <c r="Z28" s="10"/>
       <c r="AA28" s="10"/>
@@ -4605,8 +4720,10 @@
       <c r="AD28" s="10"/>
       <c r="AE28" s="10"/>
       <c r="AF28" s="10"/>
+      <c r="AG28" s="10"/>
+      <c r="AH28" s="10"/>
     </row>
-    <row r="29" spans="1:32" ht="102" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>89</v>
       </c>
@@ -4647,16 +4764,16 @@
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
-      <c r="S29" s="16" t="s">
+      <c r="S29" s="14"/>
+      <c r="T29" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T29" s="16" t="s">
+      <c r="U29" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="U29" s="14"/>
       <c r="V29" s="14"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="14"/>
+      <c r="W29" s="14"/>
+      <c r="X29" s="15"/>
       <c r="Y29" s="14"/>
       <c r="Z29" s="14"/>
       <c r="AA29" s="14"/>
@@ -4665,8 +4782,10 @@
       <c r="AD29" s="14"/>
       <c r="AE29" s="14"/>
       <c r="AF29" s="14"/>
+      <c r="AG29" s="14"/>
+      <c r="AH29" s="14"/>
     </row>
-    <row r="30" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>14</v>
       </c>
@@ -4705,16 +4824,16 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="14"/>
       <c r="R30" s="14"/>
-      <c r="S30" s="16" t="s">
+      <c r="S30" s="14"/>
+      <c r="T30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T30" s="16" t="s">
+      <c r="U30" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="U30" s="14"/>
       <c r="V30" s="14"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="14"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="15"/>
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
       <c r="AA30" s="14"/>
@@ -4723,8 +4842,10 @@
       <c r="AD30" s="14"/>
       <c r="AE30" s="14"/>
       <c r="AF30" s="14"/>
+      <c r="AG30" s="14"/>
+      <c r="AH30" s="14"/>
     </row>
-    <row r="31" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>15</v>
       </c>
@@ -4763,16 +4884,16 @@
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
-      <c r="S31" s="16" t="s">
+      <c r="S31" s="14"/>
+      <c r="T31" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T31" s="16" t="s">
+      <c r="U31" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="U31" s="14"/>
       <c r="V31" s="14"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="15"/>
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
       <c r="AA31" s="14"/>
@@ -4781,8 +4902,10 @@
       <c r="AD31" s="14"/>
       <c r="AE31" s="14"/>
       <c r="AF31" s="14"/>
+      <c r="AG31" s="14"/>
+      <c r="AH31" s="14"/>
     </row>
-    <row r="32" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>142</v>
       </c>
@@ -4811,22 +4934,22 @@
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="18"/>
-      <c r="S32" s="16" t="s">
+      <c r="S32" s="18"/>
+      <c r="T32" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T32" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="U32" s="14" t="s">
+      <c r="U32" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V32" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W32" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="X32" s="14"/>
+      <c r="W32" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X32" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
       <c r="AA32" s="14"/>
@@ -4835,8 +4958,10 @@
       <c r="AD32" s="14"/>
       <c r="AE32" s="14"/>
       <c r="AF32" s="14"/>
+      <c r="AG32" s="14"/>
+      <c r="AH32" s="14"/>
     </row>
-    <row r="33" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>146</v>
       </c>
@@ -4865,22 +4990,22 @@
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
       <c r="R33" s="18"/>
-      <c r="S33" s="16" t="s">
+      <c r="S33" s="18"/>
+      <c r="T33" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T33" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="U33" s="14" t="s">
+      <c r="U33" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V33" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W33" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="X33" s="14"/>
+      <c r="W33" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X33" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="Y33" s="14"/>
       <c r="Z33" s="14"/>
       <c r="AA33" s="14"/>
@@ -4889,8 +5014,10 @@
       <c r="AD33" s="14"/>
       <c r="AE33" s="14"/>
       <c r="AF33" s="14"/>
+      <c r="AG33" s="14"/>
+      <c r="AH33" s="14"/>
     </row>
-    <row r="34" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>143</v>
       </c>
@@ -4919,22 +5046,22 @@
       <c r="P34" s="18"/>
       <c r="Q34" s="18"/>
       <c r="R34" s="18"/>
-      <c r="S34" s="16" t="s">
+      <c r="S34" s="18"/>
+      <c r="T34" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T34" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="U34" s="14" t="s">
+      <c r="U34" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V34" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W34" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="X34" s="14"/>
+      <c r="W34" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X34" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="Y34" s="14"/>
       <c r="Z34" s="14"/>
       <c r="AA34" s="14"/>
@@ -4943,8 +5070,10 @@
       <c r="AD34" s="14"/>
       <c r="AE34" s="14"/>
       <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
     </row>
-    <row r="35" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>144</v>
       </c>
@@ -4973,22 +5102,22 @@
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="18"/>
-      <c r="S35" s="16" t="s">
+      <c r="S35" s="18"/>
+      <c r="T35" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T35" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="U35" s="14" t="s">
+      <c r="U35" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W35" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="X35" s="14"/>
+      <c r="W35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X35" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
       <c r="AA35" s="14"/>
@@ -4997,8 +5126,10 @@
       <c r="AD35" s="14"/>
       <c r="AE35" s="14"/>
       <c r="AF35" s="14"/>
+      <c r="AG35" s="14"/>
+      <c r="AH35" s="14"/>
     </row>
-    <row r="36" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>145</v>
       </c>
@@ -5027,22 +5158,22 @@
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
       <c r="R36" s="18"/>
-      <c r="S36" s="16" t="s">
+      <c r="S36" s="18"/>
+      <c r="T36" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="T36" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="U36" s="14" t="s">
+      <c r="U36" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V36" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W36" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="X36" s="14"/>
+      <c r="W36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X36" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="Y36" s="14"/>
       <c r="Z36" s="14"/>
       <c r="AA36" s="14"/>
@@ -5051,8 +5182,10 @@
       <c r="AD36" s="14"/>
       <c r="AE36" s="14"/>
       <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
+      <c r="AH36" s="14"/>
     </row>
-    <row r="37" spans="1:32" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="40" t="s">
         <v>107</v>
       </c>
@@ -5081,16 +5214,16 @@
       <c r="P37" s="18"/>
       <c r="Q37" s="18"/>
       <c r="R37" s="18"/>
-      <c r="S37" s="44" t="s">
+      <c r="S37" s="18"/>
+      <c r="T37" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="T37" s="47" t="s">
+      <c r="U37" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="U37" s="35"/>
       <c r="V37" s="35"/>
-      <c r="W37" s="54"/>
-      <c r="X37" s="35"/>
+      <c r="W37" s="35"/>
+      <c r="X37" s="54"/>
       <c r="Y37" s="35"/>
       <c r="Z37" s="35"/>
       <c r="AA37" s="35"/>
@@ -5099,8 +5232,10 @@
       <c r="AD37" s="35"/>
       <c r="AE37" s="35"/>
       <c r="AF37" s="35"/>
+      <c r="AG37" s="35"/>
+      <c r="AH37" s="35"/>
     </row>
-    <row r="38" spans="1:32" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="40" t="s">
         <v>16</v>
       </c>
@@ -5131,22 +5266,22 @@
       <c r="P38" s="18"/>
       <c r="Q38" s="18"/>
       <c r="R38" s="18"/>
-      <c r="S38" s="44" t="s">
+      <c r="S38" s="18"/>
+      <c r="T38" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="T38" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="U38" s="48" t="s">
+      <c r="U38" s="47" t="s">
         <v>2</v>
       </c>
       <c r="V38" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="W38" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="X38" s="48"/>
+      <c r="W38" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="X38" s="49" t="s">
+        <v>2</v>
+      </c>
       <c r="Y38" s="48"/>
       <c r="Z38" s="48"/>
       <c r="AA38" s="48"/>
@@ -5155,8 +5290,10 @@
       <c r="AD38" s="48"/>
       <c r="AE38" s="48"/>
       <c r="AF38" s="48"/>
+      <c r="AG38" s="48"/>
+      <c r="AH38" s="48"/>
     </row>
-    <row r="39" spans="1:32" ht="170" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="40" t="s">
         <v>90</v>
       </c>
@@ -5187,22 +5324,22 @@
       <c r="P39" s="18"/>
       <c r="Q39" s="18"/>
       <c r="R39" s="18"/>
-      <c r="S39" s="44" t="s">
+      <c r="S39" s="18"/>
+      <c r="T39" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="T39" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="U39" s="40" t="s">
+      <c r="U39" s="44" t="s">
         <v>17</v>
       </c>
       <c r="V39" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="W39" s="41" t="s">
+      <c r="W39" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="X39" s="40"/>
+      <c r="X39" s="41" t="s">
+        <v>17</v>
+      </c>
       <c r="Y39" s="40"/>
       <c r="Z39" s="40"/>
       <c r="AA39" s="40"/>
@@ -5211,8 +5348,10 @@
       <c r="AD39" s="40"/>
       <c r="AE39" s="40"/>
       <c r="AF39" s="40"/>
+      <c r="AG39" s="40"/>
+      <c r="AH39" s="40"/>
     </row>
-    <row r="40" spans="1:32" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40" t="s">
         <v>19</v>
       </c>
@@ -5247,22 +5386,22 @@
       <c r="P40" s="40"/>
       <c r="Q40" s="40"/>
       <c r="R40" s="40"/>
-      <c r="S40" s="44" t="s">
+      <c r="S40" s="40"/>
+      <c r="T40" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="T40" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="U40" s="51" t="s">
+      <c r="U40" s="50" t="s">
         <v>2</v>
       </c>
       <c r="V40" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="W40" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="X40" s="51"/>
+      <c r="W40" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="X40" s="52" t="s">
+        <v>2</v>
+      </c>
       <c r="Y40" s="51"/>
       <c r="Z40" s="51"/>
       <c r="AA40" s="51"/>
@@ -5271,8 +5410,10 @@
       <c r="AD40" s="51"/>
       <c r="AE40" s="51"/>
       <c r="AF40" s="51"/>
+      <c r="AG40" s="51"/>
+      <c r="AH40" s="51"/>
     </row>
-    <row r="41" spans="1:32" ht="40" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" ht="40" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="40" t="s">
         <v>21</v>
       </c>
@@ -5305,22 +5446,22 @@
       <c r="P41" s="40"/>
       <c r="Q41" s="40"/>
       <c r="R41" s="40"/>
-      <c r="S41" s="44" t="s">
+      <c r="S41" s="40"/>
+      <c r="T41" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="T41" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="U41" s="40" t="s">
+      <c r="U41" s="44" t="s">
         <v>2</v>
       </c>
       <c r="V41" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="W41" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="X41" s="40"/>
+      <c r="W41" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="X41" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="Y41" s="40"/>
       <c r="Z41" s="40"/>
       <c r="AA41" s="40"/>
@@ -5329,8 +5470,10 @@
       <c r="AD41" s="40"/>
       <c r="AE41" s="40"/>
       <c r="AF41" s="40"/>
+      <c r="AG41" s="40"/>
+      <c r="AH41" s="40"/>
     </row>
-    <row r="42" spans="1:32" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="40" t="s">
         <v>40</v>
       </c>
@@ -5363,22 +5506,22 @@
       <c r="P42" s="40"/>
       <c r="Q42" s="40"/>
       <c r="R42" s="40"/>
-      <c r="S42" s="44" t="s">
+      <c r="S42" s="40"/>
+      <c r="T42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="T42" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="U42" s="40" t="s">
+      <c r="U42" s="44" t="s">
         <v>2</v>
       </c>
       <c r="V42" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="W42" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="X42" s="40"/>
+      <c r="W42" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="X42" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="Y42" s="40"/>
       <c r="Z42" s="40"/>
       <c r="AA42" s="40"/>
@@ -5387,8 +5530,10 @@
       <c r="AD42" s="40"/>
       <c r="AE42" s="40"/>
       <c r="AF42" s="40"/>
+      <c r="AG42" s="40"/>
+      <c r="AH42" s="40"/>
     </row>
-    <row r="43" spans="1:32" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="40" t="s">
         <v>41</v>
       </c>
@@ -5421,22 +5566,22 @@
       <c r="P43" s="40"/>
       <c r="Q43" s="40"/>
       <c r="R43" s="40"/>
-      <c r="S43" s="44" t="s">
+      <c r="S43" s="40"/>
+      <c r="T43" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="T43" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="U43" s="40" t="s">
+      <c r="U43" s="44" t="s">
         <v>2</v>
       </c>
       <c r="V43" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="W43" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="X43" s="40"/>
+      <c r="W43" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="X43" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="Y43" s="40"/>
       <c r="Z43" s="40"/>
       <c r="AA43" s="40"/>
@@ -5445,8 +5590,10 @@
       <c r="AD43" s="40"/>
       <c r="AE43" s="40"/>
       <c r="AF43" s="40"/>
+      <c r="AG43" s="40"/>
+      <c r="AH43" s="40"/>
     </row>
-    <row r="44" spans="1:32" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
         <v>42</v>
       </c>
@@ -5479,22 +5626,22 @@
       <c r="P44" s="40"/>
       <c r="Q44" s="40"/>
       <c r="R44" s="40"/>
-      <c r="S44" s="44" t="s">
+      <c r="S44" s="40"/>
+      <c r="T44" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="T44" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="U44" s="40" t="s">
+      <c r="U44" s="44" t="s">
         <v>2</v>
       </c>
       <c r="V44" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="W44" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="X44" s="40"/>
+      <c r="W44" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="X44" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="Y44" s="40"/>
       <c r="Z44" s="40"/>
       <c r="AA44" s="40"/>
@@ -5503,8 +5650,10 @@
       <c r="AD44" s="40"/>
       <c r="AE44" s="40"/>
       <c r="AF44" s="40"/>
+      <c r="AG44" s="40"/>
+      <c r="AH44" s="40"/>
     </row>
-    <row r="45" spans="1:32" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="40" t="s">
         <v>43</v>
       </c>
@@ -5537,22 +5686,22 @@
       <c r="P45" s="40"/>
       <c r="Q45" s="40"/>
       <c r="R45" s="40"/>
-      <c r="S45" s="44" t="s">
+      <c r="S45" s="40"/>
+      <c r="T45" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="T45" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="U45" s="40" t="s">
+      <c r="U45" s="44" t="s">
         <v>2</v>
       </c>
       <c r="V45" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="W45" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="X45" s="40"/>
+      <c r="W45" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="X45" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="Y45" s="40"/>
       <c r="Z45" s="40"/>
       <c r="AA45" s="40"/>
@@ -5561,8 +5710,10 @@
       <c r="AD45" s="40"/>
       <c r="AE45" s="40"/>
       <c r="AF45" s="40"/>
+      <c r="AG45" s="40"/>
+      <c r="AH45" s="40"/>
     </row>
-    <row r="46" spans="1:32" ht="276" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" ht="276" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>78</v>
       </c>
@@ -5611,52 +5762,54 @@
       <c r="P46" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="Q46" s="31" t="s">
+      <c r="Q46" s="6"/>
+      <c r="R46" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="R46" s="6" t="s">
+      <c r="S46" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="S46" s="8" t="s">
+      <c r="T46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T46" s="20"/>
-      <c r="U46" s="6" t="s">
+      <c r="U46" s="20"/>
+      <c r="V46" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="V46" s="6" t="s">
+      <c r="W46" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="W46" s="6" t="s">
+      <c r="X46" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="X46" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="Y46" s="6" t="s">
         <v>206</v>
       </c>
       <c r="Z46" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA46" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="AA46" s="6" t="s">
+      <c r="AB46" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="AB46" s="6" t="s">
+      <c r="AC46" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="AC46" s="6" t="s">
+      <c r="AD46" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="AD46" s="6" t="s">
+      <c r="AE46" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="AE46" s="6"/>
-      <c r="AF46" s="6" t="s">
+      <c r="AF46" s="6"/>
+      <c r="AG46" s="6"/>
+      <c r="AH46" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>98</v>
       </c>
@@ -5685,24 +5838,24 @@
       <c r="N47" s="18"/>
       <c r="O47" s="18"/>
       <c r="P47" s="18"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="8" t="s">
+      <c r="Q47" s="18"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T47" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U47" s="6" t="s">
+      <c r="U47" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V47" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W47" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X47" s="6"/>
+      <c r="W47" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y47" s="6"/>
       <c r="Z47" s="6"/>
       <c r="AA47" s="6"/>
@@ -5711,8 +5864,10 @@
       <c r="AD47" s="6"/>
       <c r="AE47" s="6"/>
       <c r="AF47" s="6"/>
+      <c r="AG47" s="6"/>
+      <c r="AH47" s="6"/>
     </row>
-    <row r="48" spans="1:32" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>99</v>
       </c>
@@ -5741,24 +5896,24 @@
       <c r="N48" s="18"/>
       <c r="O48" s="18"/>
       <c r="P48" s="18"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="8" t="s">
+      <c r="Q48" s="18"/>
+      <c r="R48" s="31"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T48" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U48" s="6" t="s">
+      <c r="U48" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V48" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W48" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X48" s="6"/>
+      <c r="W48" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X48" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y48" s="6"/>
       <c r="Z48" s="6"/>
       <c r="AA48" s="6"/>
@@ -5767,8 +5922,10 @@
       <c r="AD48" s="6"/>
       <c r="AE48" s="6"/>
       <c r="AF48" s="6"/>
+      <c r="AG48" s="6"/>
+      <c r="AH48" s="6"/>
     </row>
-    <row r="49" spans="1:32" ht="227" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" ht="227" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>100</v>
       </c>
@@ -5817,52 +5974,54 @@
       <c r="P49" s="61" t="s">
         <v>232</v>
       </c>
-      <c r="Q49" s="70" t="s">
+      <c r="Q49" s="61"/>
+      <c r="R49" s="70" t="s">
         <v>256</v>
       </c>
-      <c r="R49" s="61" t="s">
+      <c r="S49" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="S49" s="8" t="s">
+      <c r="T49" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T49" s="20"/>
-      <c r="U49" s="6" t="s">
+      <c r="U49" s="20"/>
+      <c r="V49" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="V49" s="6" t="s">
+      <c r="W49" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="W49" s="6" t="s">
+      <c r="X49" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="X49" s="6" t="s">
+      <c r="Y49" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="Y49" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="Z49" s="6" t="s">
         <v>207</v>
       </c>
       <c r="AA49" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB49" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="AB49" s="6" t="s">
+      <c r="AC49" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AC49" s="6" t="s">
+      <c r="AD49" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="AD49" s="6" t="s">
+      <c r="AE49" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AE49" s="6"/>
-      <c r="AF49" s="6" t="s">
+      <c r="AF49" s="6"/>
+      <c r="AG49" s="6"/>
+      <c r="AH49" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="50" spans="1:32" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>156</v>
       </c>
@@ -5893,22 +6052,22 @@
       <c r="P50" s="18"/>
       <c r="Q50" s="18"/>
       <c r="R50" s="18"/>
-      <c r="S50" s="8" t="s">
+      <c r="S50" s="18"/>
+      <c r="T50" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T50" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U50" s="6" t="s">
+      <c r="U50" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V50" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W50" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X50" s="6"/>
+      <c r="W50" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X50" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y50" s="6"/>
       <c r="Z50" s="6"/>
       <c r="AA50" s="6"/>
@@ -5917,8 +6076,10 @@
       <c r="AD50" s="6"/>
       <c r="AE50" s="6"/>
       <c r="AF50" s="6"/>
+      <c r="AG50" s="6"/>
+      <c r="AH50" s="6"/>
     </row>
-    <row r="51" spans="1:32" ht="153" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
@@ -5967,27 +6128,25 @@
       <c r="P51" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="Q51" s="31" t="s">
+      <c r="Q51" s="6"/>
+      <c r="R51" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="R51" s="6" t="s">
+      <c r="S51" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="S51" s="8" t="s">
+      <c r="T51" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T51" s="20"/>
-      <c r="U51" s="6" t="s">
+      <c r="U51" s="20"/>
+      <c r="V51" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="V51" s="6" t="s">
+      <c r="W51" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="W51" s="6" t="s">
+      <c r="X51" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="X51" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="Y51" s="6" t="s">
         <v>199</v>
@@ -6007,12 +6166,16 @@
       <c r="AD51" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AE51" s="6"/>
-      <c r="AF51" s="6" t="s">
+      <c r="AE51" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF51" s="6"/>
+      <c r="AG51" s="6"/>
+      <c r="AH51" s="6" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
@@ -6061,27 +6224,25 @@
       <c r="P52" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="Q52" s="31" t="s">
+      <c r="Q52" s="6"/>
+      <c r="R52" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="R52" s="6" t="s">
+      <c r="S52" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="S52" s="8" t="s">
+      <c r="T52" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T52" s="20"/>
-      <c r="U52" s="6" t="s">
+      <c r="U52" s="20"/>
+      <c r="V52" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="V52" s="6" t="s">
+      <c r="W52" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="W52" s="6" t="s">
+      <c r="X52" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="X52" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="Y52" s="6" t="s">
         <v>199</v>
@@ -6101,10 +6262,14 @@
       <c r="AD52" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AE52" s="6"/>
+      <c r="AE52" s="6" t="s">
+        <v>199</v>
+      </c>
       <c r="AF52" s="6"/>
+      <c r="AG52" s="6"/>
+      <c r="AH52" s="6"/>
     </row>
-    <row r="53" spans="1:32" ht="272" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" ht="272" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>175</v>
       </c>
@@ -6153,32 +6318,30 @@
       <c r="P53" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="Q53" s="31" t="s">
+      <c r="Q53" s="6"/>
+      <c r="R53" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="R53" s="61" t="s">
+      <c r="S53" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="S53" s="8"/>
-      <c r="T53" s="20"/>
-      <c r="U53" s="6" t="s">
-        <v>179</v>
-      </c>
+      <c r="T53" s="8"/>
+      <c r="U53" s="20"/>
       <c r="V53" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W53" s="32"/>
-      <c r="X53" s="6" t="s">
+      <c r="W53" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="X53" s="32"/>
+      <c r="Y53" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="Y53" s="6" t="s">
+      <c r="Z53" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="Z53" s="6" t="s">
+      <c r="AA53" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="AA53" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="AB53" s="6" t="s">
         <v>222</v>
@@ -6187,14 +6350,18 @@
         <v>222</v>
       </c>
       <c r="AD53" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE53" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="AE53" s="6"/>
-      <c r="AF53" s="6" t="s">
+      <c r="AF53" s="6"/>
+      <c r="AG53" s="6"/>
+      <c r="AH53" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="54" spans="1:32" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>174</v>
       </c>
@@ -6223,24 +6390,24 @@
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
-      <c r="Q54" s="31"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="8" t="s">
+      <c r="Q54" s="6"/>
+      <c r="R54" s="31"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T54" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U54" s="6" t="s">
+      <c r="U54" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V54" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W54" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X54" s="6"/>
+      <c r="W54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X54" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y54" s="6"/>
       <c r="Z54" s="6"/>
       <c r="AA54" s="6"/>
@@ -6249,8 +6416,10 @@
       <c r="AD54" s="6"/>
       <c r="AE54" s="6"/>
       <c r="AF54" s="6"/>
+      <c r="AG54" s="6"/>
+      <c r="AH54" s="6"/>
     </row>
-    <row r="55" spans="1:32" ht="136" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>10</v>
       </c>
@@ -6299,27 +6468,25 @@
       <c r="P55" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="Q55" s="31" t="s">
+      <c r="Q55" s="6"/>
+      <c r="R55" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="R55" s="6" t="s">
+      <c r="S55" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="S55" s="8" t="s">
+      <c r="T55" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T55" s="20"/>
-      <c r="U55" s="6" t="s">
+      <c r="U55" s="20"/>
+      <c r="V55" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="V55" s="6" t="s">
+      <c r="W55" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="W55" s="6" t="s">
+      <c r="X55" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="X55" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="Y55" s="6" t="s">
         <v>202</v>
@@ -6339,12 +6506,16 @@
       <c r="AD55" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AE55" s="6"/>
-      <c r="AF55" s="6" t="s">
+      <c r="AE55" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF55" s="6"/>
+      <c r="AG55" s="6"/>
+      <c r="AH55" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>11</v>
       </c>
@@ -6373,22 +6544,22 @@
       <c r="P56" s="18"/>
       <c r="Q56" s="18"/>
       <c r="R56" s="18"/>
-      <c r="S56" s="58" t="s">
+      <c r="S56" s="18"/>
+      <c r="T56" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="T56" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U56" s="6" t="s">
+      <c r="U56" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V56" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W56" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X56" s="6"/>
+      <c r="W56" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y56" s="6"/>
       <c r="Z56" s="6"/>
       <c r="AA56" s="6"/>
@@ -6397,8 +6568,10 @@
       <c r="AD56" s="6"/>
       <c r="AE56" s="6"/>
       <c r="AF56" s="6"/>
+      <c r="AG56" s="6"/>
+      <c r="AH56" s="6"/>
     </row>
-    <row r="57" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>12</v>
       </c>
@@ -6427,22 +6600,22 @@
       <c r="P57" s="18"/>
       <c r="Q57" s="18"/>
       <c r="R57" s="18"/>
-      <c r="S57" s="58" t="s">
+      <c r="S57" s="18"/>
+      <c r="T57" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="T57" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U57" s="6" t="s">
+      <c r="U57" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V57" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W57" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X57" s="6"/>
+      <c r="W57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y57" s="6"/>
       <c r="Z57" s="6"/>
       <c r="AA57" s="6"/>
@@ -6451,8 +6624,10 @@
       <c r="AD57" s="6"/>
       <c r="AE57" s="6"/>
       <c r="AF57" s="6"/>
+      <c r="AG57" s="6"/>
+      <c r="AH57" s="6"/>
     </row>
-    <row r="58" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>13</v>
       </c>
@@ -6481,22 +6656,22 @@
       <c r="P58" s="18"/>
       <c r="Q58" s="18"/>
       <c r="R58" s="18"/>
-      <c r="S58" s="58" t="s">
+      <c r="S58" s="18"/>
+      <c r="T58" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="T58" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U58" s="6" t="s">
+      <c r="U58" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V58" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W58" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X58" s="6"/>
+      <c r="W58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X58" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="Y58" s="6"/>
       <c r="Z58" s="6"/>
       <c r="AA58" s="6"/>
@@ -6505,8 +6680,10 @@
       <c r="AD58" s="6"/>
       <c r="AE58" s="6"/>
       <c r="AF58" s="6"/>
+      <c r="AG58" s="6"/>
+      <c r="AH58" s="6"/>
     </row>
-    <row r="59" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>84</v>
       </c>
@@ -6534,9 +6711,6 @@
       <c r="I59" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="S59" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="T59" s="5" t="s">
         <v>84</v>
       </c>
@@ -6547,6 +6721,9 @@
         <v>84</v>
       </c>
       <c r="W59" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="X59" s="5" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unlinked all trate priors
</commit_message>
<xml_diff>
--- a/documentation/PARAMS.xlsx
+++ b/documentation/PARAMS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFFA4E9-2B72-6F49-8DD9-37F1BB25793B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4787333D-886C-DF43-AEF0-A3725053228B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38380" windowHeight="19560" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
+    <workbookView xWindow="19400" yWindow="500" windowWidth="18980" windowHeight="19560" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="301">
   <si>
     <t>Parameter</t>
   </si>
@@ -746,235 +746,6 @@
       </rPr>
       <t xml:space="preserve"> 
 Calculated from AIDS Info data: total AIDS-related deaths/ total HIV prevalence</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trate.0 (1990) = 8 * trate.1
-Trate.1 (1997) = 1 * trate.2
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 1 * trate.2
-Trate.4 (2030) = 1 *  trate.3
-SD of r0:r1 ratio = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>log(2)/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SD of r1:r2 ratio = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>log(2)/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SD of r2 = log(4)/2
-SD of r3:r2 ratio = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>log(2)/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SD of r4:r3 ratio = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>log(2)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trate.0 (1990) = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * trate.1
-Trate.1 (1997) = 1 * trate.2
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 1 * trate.2
-Trate.4 (2030) = 1 *  trate.3
-SD of r0:r1 ratio = log(4)/2
-SD of r1:r2 ratio = log(4)/2
-SD of r2 = log(4)/2
-SD of r3:r2 ratio = log(4)/2
-SD of r4:r3 ratio = log(4)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Trate.0 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1980</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * trate.1
-Trate.1 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>1993</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.75</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * trate.2
-Trate.2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2005</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) = 0.1
-Trate.3 (2018) = 1 * trate.2
-Trate.4 (2030) = 1 *  trate.3
-SD of r0:r1 ratio = log(4)/2
-SD of r1:r2 ratio = log(4)/2
-SD of r2 = log(4)/2
-SD of r3:r2 ratio = log(4)/2
-SD of r4:r3 ratio = log(4)/2</t>
     </r>
   </si>
   <si>
@@ -1160,18 +931,6 @@
     <t>DHS 2003, 2011, 2022 - see "DHS_tables.xlsx"</t>
   </si>
   <si>
-    <t>Trate.0 (1990) = 8 * trate.1
-Trate.1 (1997) = 1 * trate.2
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 1 * trate.2
-Trate.4 (2030) = 1 *  trate.3
-SD of r0:r1 ratio = log(4)/2
-SD of r1:r2 ratio = log(4)/2
-SD of r2 = log(4)/2
-SD of r3:r2 ratio = log(4)/2
-SD of r4:r3 ratio = log(4)/2</t>
-  </si>
-  <si>
     <t>Tanzania</t>
   </si>
   <si>
@@ -1468,77 +1227,10 @@
     <t>Using SOUTH AFRICA suppression data (IeDEA dashboard for West Africa missing a lot of data; values seem close enough to SA)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Trate.0 (1990) = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6.5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * trate.1
-Trate.1 (1997) = 1 * trate.2
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 1 * trate.2
-Trate.4 (2030) = 1 *  trate.3
-SD of r0:r1 ratio = log(4)/2
-SD of r1:r2 ratio = log(4)/2
-SD of r2 = log(4)/2
-SD of r3:r2 ratio = log(4)/2
-SD of r4:r3 ratio = log(4)/2</t>
-    </r>
-  </si>
-  <si>
     <t>UNAIDS remainder</t>
   </si>
   <si>
     <t>Non-UNAIDS remainder</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trate.0 (1990) = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * trate.1
-Trate.1 (1997) = 1 * trate.2
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 1 * trate.2
-Trate.4 (2030) = 1 *  trate.3
-SD of r0:r1 ratio = log(4)/2
-SD of r1:r2 ratio = log(4)/2
-SD of r2 = log(4)/2
-SD of r3:r2 ratio = log(4)/2
-SD of r4:r3 ratio = log(4)/2</t>
-    </r>
   </si>
   <si>
     <t>Using KENYA'S suppression data</t>
@@ -2087,12 +1779,351 @@
   <si>
     <t>Barennes, 2014</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UNLINKED:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.8
+Trate.1 (1997) = 0.1
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OLD VERSION:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trate.0 (1990) = 8 * trate.1
+Trate.1 (1997) = 1 * trate.2
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 1 * trate.2
+Trate.4 (2030) = 1 *  trate.3
+SD of r0:r1 ratio = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log(2)/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SD of r1:r2 ratio = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log(2)/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SD of r2 = log(4)/2
+SD of r3:r2 ratio = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log(2)/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SD of r4:r3 ratio = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log(2)/2</t>
+    </r>
+  </si>
+  <si>
+    <t>UNLINKED:
+Trate.0 (1990) = 0.8
+Trate.1 (1997) = 0.1
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+Trate.0 (1990) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trate.1 (1997) = 0.1
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.5
+Trate.1 (1997) = 0.12
+Trate.2 (2008) = 0.12
+Trate.3 (2018) = 0.12
+Trate.4 (2030) = 0.15
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>UNLINKED:
+Trate.0 (1990) =</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trate.1 (1997) = 0.1
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.65
+Trate.1 (1997) = 0.06
+Trate.2 (2008) = 0.06
+Trate.3 (2018) = 0.06
+Trate.4 (2030) = 0.06
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.47
+Trate.1 (1997) = 0.06
+Trate.2 (2008) = 0.06
+Trate.3 (2018) = 0.06
+Trate.4 (2030) = 0.06
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.41
+Trate.1 (1997) = 0.45
+Trate.2 (2008) = 0.15
+Trate.3 (2018) = 0.12
+Trate.4 (2030) = 0.12
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2139,12 +2170,6 @@
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow (Body)"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
@@ -2544,28 +2569,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2941,10 +2966,10 @@
   <dimension ref="A1:AJ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3037,37 +3062,37 @@
         <v>24</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K2" s="63" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="L2" s="63" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="M2" s="63" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="N2" s="63" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O2" s="63" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="P2" s="63" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Q2" s="63" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="R2" s="63" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="S2" s="63" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="T2" s="63" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="U2" s="63"/>
       <c r="V2" s="62" t="s">
@@ -3083,37 +3108,37 @@
         <v>24</v>
       </c>
       <c r="Z2" s="65" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AA2" s="65" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AB2" s="65" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AC2" s="65" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="AD2" s="65" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AE2" s="65" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="AF2" s="65" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AG2" s="65" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="AH2" s="65" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AI2" s="63" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AJ2" s="63" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="211" customHeight="1" x14ac:dyDescent="0.2">
@@ -3131,49 +3156,49 @@
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="P3" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="R3" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="S3" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="T3" s="25" t="s">
-        <v>236</v>
+        <v>167</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>300</v>
       </c>
       <c r="U3" s="26"/>
       <c r="V3" s="26" t="s">
@@ -3278,46 +3303,46 @@
         <v>153</v>
       </c>
       <c r="G5" s="55" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H5" s="55" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J5" s="55" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K5" s="55" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="L5" s="55" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M5" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="N5" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="O5" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="N5" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="O5" s="55" t="s">
-        <v>226</v>
-      </c>
       <c r="P5" s="55" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="Q5" s="55" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="R5" s="55" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="S5" s="55" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="T5" s="55" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="U5" s="30" t="s">
         <v>5</v>
@@ -3330,40 +3355,40 @@
         <v>152</v>
       </c>
       <c r="Y5" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Z5" s="55" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="AA5" s="55" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="AB5" s="55" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AC5" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD5" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE5" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="AD5" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="AE5" s="55" t="s">
-        <v>226</v>
-      </c>
       <c r="AF5" s="55" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AG5" s="55" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="AH5" s="55" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="AI5" s="55" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AJ5" s="55" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="85" x14ac:dyDescent="0.2">
@@ -3436,40 +3461,40 @@
         <v>152</v>
       </c>
       <c r="Y6" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Z6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AA6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AB6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AC6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AD6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AE6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AF6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AG6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AH6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AI6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AJ6" s="55" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
@@ -3780,19 +3805,19 @@
         <v>32</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>49</v>
       </c>
       <c r="G12" s="59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H12" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I12" s="73" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J12" s="27" t="s">
         <v>83</v>
@@ -3816,58 +3841,58 @@
         <v>83</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="R12" s="31"/>
       <c r="S12" s="71" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="T12" s="71" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="U12" s="30" t="s">
         <v>5</v>
       </c>
       <c r="V12" s="20"/>
       <c r="W12" s="27" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="X12" s="27" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Y12" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="Z12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AA12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AB12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AC12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AD12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AE12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AF12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AG12" s="25" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="AH12" s="25"/>
       <c r="AI12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AJ12" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="119" hidden="1" x14ac:dyDescent="0.2">
@@ -3944,7 +3969,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="27">
@@ -3954,7 +3979,7 @@
         <v>0.42</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="J14" s="27">
         <v>0.42</v>
@@ -3978,16 +4003,16 @@
         <v>0.42</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="S14" s="71" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="T14" s="71" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="U14" s="30" t="s">
         <v>9</v>
@@ -4024,10 +4049,10 @@
         <v>60</v>
       </c>
       <c r="AG14" s="25" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="AH14" s="25" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="AI14" s="25" t="s">
         <v>60</v>
@@ -4106,7 +4131,7 @@
         <v>32</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>113</v>
@@ -4874,7 +4899,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>31</v>
@@ -4895,10 +4920,10 @@
         <v>5.3571430000000003E-2</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
@@ -4938,7 +4963,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>31</v>
@@ -4957,10 +4982,10 @@
         <v>2.272727E-3</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
@@ -5000,7 +5025,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>31</v>
@@ -5019,10 +5044,10 @@
         <v>3.9473679999999997E-3</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="L31" s="14"/>
       <c r="M31" s="14"/>
@@ -5849,7 +5874,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I45" s="40"/>
       <c r="J45" s="40"/>
@@ -5904,7 +5929,7 @@
         <v>32</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>84</v>
@@ -5916,40 +5941,40 @@
         <v>158</v>
       </c>
       <c r="I46" s="56" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="Q46" s="6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="S46" s="31" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="U46" s="8" t="s">
         <v>5</v>
@@ -5962,38 +5987,38 @@
         <v>151</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="Z46" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="AA46" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="AB46" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AC46" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AD46" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AE46" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AF46" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AG46" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AH46" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="AI46" s="6"/>
       <c r="AJ46" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="102" hidden="1" x14ac:dyDescent="0.2">
@@ -6130,52 +6155,52 @@
         <v>32</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G49" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="H49" s="56" t="s">
         <v>210</v>
       </c>
-      <c r="H49" s="56" t="s">
-        <v>214</v>
-      </c>
       <c r="I49" s="56" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="J49" s="61" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K49" s="61" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L49" s="61" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M49" s="61" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="N49" s="61" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="O49" s="61" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="P49" s="61" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="Q49" s="6" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="R49" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="S49" s="70" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="T49" s="61" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="U49" s="8" t="s">
         <v>5</v>
@@ -6185,41 +6210,41 @@
         <v>62</v>
       </c>
       <c r="X49" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Y49" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="Z49" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AA49" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB49" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AC49" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AD49" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AE49" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AF49" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AG49" s="6" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="AH49" s="6" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="AI49" s="6"/>
       <c r="AJ49" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:36" ht="119" hidden="1" x14ac:dyDescent="0.2">
@@ -6290,13 +6315,13 @@
         <v>36</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>85</v>
@@ -6308,40 +6333,40 @@
         <v>0.15548490000000001</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="P51" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="Q51" s="61" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="R51" s="6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="S51" s="31" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="U51" s="8" t="s">
         <v>3</v>
@@ -6351,41 +6376,41 @@
         <v>63</v>
       </c>
       <c r="X51" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Y51" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="Z51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AA51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AB51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AC51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AD51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AE51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AF51" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AG51" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="AH51" s="6" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="AI51" s="6"/>
       <c r="AJ51" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:36" ht="51" x14ac:dyDescent="0.2">
@@ -6396,13 +6421,13 @@
         <v>36</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>85</v>
@@ -6414,40 +6439,40 @@
         <v>0.15548490000000001</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="Q52" s="6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="R52" s="6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="S52" s="31" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="U52" s="8" t="s">
         <v>3</v>
@@ -6457,34 +6482,34 @@
         <v>63</v>
       </c>
       <c r="X52" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="Z52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AA52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AB52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AC52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AD52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AE52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AF52" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AG52" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="AH52" s="6"/>
       <c r="AI52" s="6"/>
@@ -6492,7 +6517,7 @@
     </row>
     <row r="53" spans="1:36" ht="272" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>36</v>
@@ -6504,97 +6529,97 @@
         <v>32</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G53" s="56" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H53" s="56" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I53" s="56" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="Q53" s="6" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="R53" s="6" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="S53" s="31" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="T53" s="61" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="U53" s="8"/>
       <c r="V53" s="20"/>
       <c r="W53" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="X53" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Y53" s="32"/>
       <c r="Z53" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AA53" s="6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AB53" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="AC53" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AD53" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AE53" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AF53" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AG53" s="6" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="AH53" s="6" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="AI53" s="6"/>
       <c r="AJ53" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>36</v>
@@ -6606,7 +6631,7 @@
         <v>31</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>156</v>
@@ -6660,13 +6685,13 @@
         <v>36</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>85</v>
@@ -6678,84 +6703,84 @@
         <v>7.5484389999999998E-2</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="Q55" s="6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="S55" s="31" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="U55" s="8" t="s">
         <v>3</v>
       </c>
       <c r="V55" s="20"/>
       <c r="W55" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="X55" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y55" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="Z55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AA55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AB55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AC55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AD55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AE55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AF55" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AG55" s="6" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="AH55" s="6" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="AI55" s="6"/>
       <c r="AJ55" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">
@@ -6790,7 +6815,7 @@
       <c r="S56" s="18"/>
       <c r="T56" s="18"/>
       <c r="U56" s="58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="V56" s="8" t="s">
         <v>2</v>
@@ -6848,7 +6873,7 @@
       <c r="S57" s="18"/>
       <c r="T57" s="18"/>
       <c r="U57" s="58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="V57" s="8" t="s">
         <v>2</v>
@@ -6906,7 +6931,7 @@
       <c r="S58" s="18"/>
       <c r="T58" s="18"/>
       <c r="U58" s="58" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V58" s="8" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
updates to remainder models
</commit_message>
<xml_diff>
--- a/documentation/PARAMS.xlsx
+++ b/documentation/PARAMS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4787333D-886C-DF43-AEF0-A3725053228B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF5E96-9124-7E49-91F7-5302D3C1C470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19400" yWindow="500" windowWidth="18980" windowHeight="19560" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
+    <workbookView xWindow="39660" yWindow="4100" windowWidth="28780" windowHeight="15540" xr2:uid="{A31A707F-ED32-BA46-921D-128043F311ED}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="300">
   <si>
     <t>Parameter</t>
   </si>
@@ -1233,9 +1233,6 @@
     <t>Non-UNAIDS remainder</t>
   </si>
   <si>
-    <t>Using KENYA'S suppression data</t>
-  </si>
-  <si>
     <t>India NFHS 2005, 2015, 2019</t>
   </si>
   <si>
@@ -1463,136 +1460,6 @@
   <si>
     <t>Estimate from India, 81.8% suppressed within 6 months (--&gt; 0.966876 within one year), Alvarez-Uria et al, 2013:
 https://onlinelibrary.wiley.com/doi/10.1155/2013/384805</t>
-  </si>
-  <si>
-    <t>Using KENYA'S testing data 
-DHS surveys from Ehtiopia, DRC, Cote d'Ivoire, Ghana; which represent ~19% of these remainder countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Global estimate of engagement from AIDSinfo data
-Using SOUTH AFRICA'S engagement data </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>ALLISON LOOK UP FOR ETHIOPIA, INDONESIA, AND DRC</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (from de Oliveira)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t xml:space="preserve">Get from JHEEM </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(from de Oliveira)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>UPDATE TO SOME AVERAGE FROM THIS PAPER</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.42
-Logitnormal
-Begins at this value in 1990, interpolates to birth.transmission.risk.1 from 1990-2020</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>UPDATE TO NYC ESTIMATE FROM THIS PAPER - 0.249</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0.42
-Logitnormal
-Begins at this value in 1990, interpolates to birth.transmission.risk.1 from 1990-2020</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1780,39 +1647,228 @@
     <t>Barennes, 2014</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UNLINKED:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Trate.0 (1990) = 0.8
+    <t>UNLINKED:
+Trate.0 (1990) = 0.8
 Trate.1 (1997) = 0.1
 Trate.2 (2008) = 0.1
 Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+Trate.0 (1990) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trate.1 (1997) = 0.1
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.5
+Trate.1 (1997) = 0.12
+Trate.2 (2008) = 0.12
+Trate.3 (2018) = 0.12
+Trate.4 (2030) = 0.15
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>UNLINKED:
+Trate.0 (1990) =</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Trate.1 (1997) = 0.1
+Trate.2 (2008) = 0.1
+Trate.3 (2018) = 0.1
+Trate.4 (2030) = 0.1
+SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.47
+Trate.1 (1997) = 0.06
+Trate.2 (2008) = 0.06
+Trate.3 (2018) = 0.06
+Trate.4 (2030) = 0.06
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.41
+Trate.1 (1997) = 0.45
+Trate.2 (2008) = 0.15
+Trate.3 (2018) = 0.12
+Trate.4 (2030) = 0.12
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UNLINKED:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.65
+Trate.1 (1997) = 0.045
+Trate.2 (2008) = 0.035
+Trate.3 (2018) = 0.03
+Trate.4 (2030) = 0.06
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SD for all = log (4)/2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UNLINKED:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Trate.0 (1990) = 0.7
+Trate.1 (1997) = 0.06
+Trate.2 (2008) = 0.08
+Trate.3 (2018) = 0.08
 Trate.4 (2030) = 0.1
 SD for all = log (4)/2
 </t>
@@ -1930,62 +1986,61 @@
     </r>
   </si>
   <si>
-    <t>UNLINKED:
-Trate.0 (1990) = 0.8
-Trate.1 (1997) = 0.1
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 0.1
-Trate.4 (2030) = 0.1
-SD for all = log (4)/2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">UNLINKED:
-Trate.0 (1990) = </t>
-    </r>
+    <t>DHS surveys from Ehtiopia, DRC, Cote d'Ivoire, Ghana; which represent ~19% of these remainder countries</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.4</t>
-    </r>
-    <r>
-      <rPr>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Actually, just keep using Kenya's 
+ALLISON LOOK UP FOR ETHIOPIA, INDONESIA, AND DRC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Trate.1 (1997) = 0.1
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 0.1
-Trate.4 (2030) = 0.1
-SD for all = log (4)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">UNLINKED:
 </t>
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (from de Oliveira)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Trate.0 (1990) = 0.5
-Trate.1 (1997) = 0.12
-Trate.2 (2008) = 0.12
-Trate.3 (2018) = 0.12
-Trate.4 (2030) = 0.15
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Actually, just keep using Kenya's 
+Get from JHEEM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1993,137 +2048,29 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SD for all = log (4)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>UNLINKED:
-Trate.0 (1990) =</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 0.65</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Trate.1 (1997) = 0.1
-Trate.2 (2008) = 0.1
-Trate.3 (2018) = 0.1
-Trate.4 (2030) = 0.1
-SD for all = log (4)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">UNLINKED:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Trate.0 (1990) = 0.65
-Trate.1 (1997) = 0.06
-Trate.2 (2008) = 0.06
-Trate.3 (2018) = 0.06
-Trate.4 (2030) = 0.06
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SD for all = log (4)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">UNLINKED:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Trate.0 (1990) = 0.47
-Trate.1 (1997) = 0.06
-Trate.2 (2008) = 0.06
-Trate.3 (2018) = 0.06
-Trate.4 (2030) = 0.06
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SD for all = log (4)/2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">UNLINKED:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Trate.0 (1990) = 0.41
-Trate.1 (1997) = 0.45
-Trate.2 (2008) = 0.15
-Trate.3 (2018) = 0.12
-Trate.4 (2030) = 0.12
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SD for all = log (4)/2</t>
-    </r>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(from de Oliveira)</t>
+    </r>
+  </si>
+  <si>
+    <t>Use Global estimate of engagement from AIDSinfo data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247
+Cote d'Ivoire estimate from Dabis paper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.249
+NYC estimate from Dabis paper </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2180,6 +2127,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2384,7 +2337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2593,16 +2546,13 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2965,11 +2915,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B2D996-732D-784F-96EB-809CE760E324}">
   <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="Q14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3083,10 +3033,10 @@
         <v>224</v>
       </c>
       <c r="Q2" s="63" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="R2" s="63" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="S2" s="63" t="s">
         <v>229</v>
@@ -3129,10 +3079,10 @@
         <v>224</v>
       </c>
       <c r="AG2" s="65" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AH2" s="65" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AI2" s="63" t="s">
         <v>229</v>
@@ -3162,43 +3112,43 @@
         <v>293</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="U3" s="26"/>
       <c r="V3" s="26" t="s">
@@ -3333,16 +3283,16 @@
         <v>225</v>
       </c>
       <c r="Q5" s="55" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="R5" s="55" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="S5" s="55" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="T5" s="55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U5" s="30" t="s">
         <v>5</v>
@@ -3379,16 +3329,16 @@
         <v>225</v>
       </c>
       <c r="AG5" s="55" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="AH5" s="55" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="AI5" s="55" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AJ5" s="55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="85" x14ac:dyDescent="0.2">
@@ -3816,7 +3766,7 @@
       <c r="H12" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="71" t="s">
         <v>181</v>
       </c>
       <c r="J12" s="27" t="s">
@@ -3841,14 +3791,14 @@
         <v>83</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="R12" s="31"/>
-      <c r="S12" s="71" t="s">
-        <v>249</v>
-      </c>
-      <c r="T12" s="71" t="s">
-        <v>250</v>
+      <c r="S12" s="55" t="s">
+        <v>295</v>
+      </c>
+      <c r="T12" s="55" t="s">
+        <v>296</v>
       </c>
       <c r="U12" s="30" t="s">
         <v>5</v>
@@ -3885,7 +3835,7 @@
         <v>184</v>
       </c>
       <c r="AG12" s="25" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="AH12" s="25"/>
       <c r="AI12" s="25" t="s">
@@ -3969,7 +3919,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="27">
@@ -3978,8 +3928,8 @@
       <c r="H14" s="27">
         <v>0.42</v>
       </c>
-      <c r="I14" s="72" t="s">
-        <v>279</v>
+      <c r="I14" s="70" t="s">
+        <v>272</v>
       </c>
       <c r="J14" s="27">
         <v>0.42</v>
@@ -4003,16 +3953,16 @@
         <v>0.42</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="S14" s="71" t="s">
-        <v>251</v>
-      </c>
-      <c r="T14" s="71" t="s">
-        <v>252</v>
+        <v>274</v>
+      </c>
+      <c r="S14" s="72" t="s">
+        <v>298</v>
+      </c>
+      <c r="T14" s="72" t="s">
+        <v>299</v>
       </c>
       <c r="U14" s="30" t="s">
         <v>9</v>
@@ -4049,10 +3999,10 @@
         <v>60</v>
       </c>
       <c r="AG14" s="25" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="AH14" s="25" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="AI14" s="25" t="s">
         <v>60</v>
@@ -5929,7 +5879,7 @@
         <v>32</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>84</v>
@@ -5941,7 +5891,7 @@
         <v>158</v>
       </c>
       <c r="I46" s="56" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>186</v>
@@ -5965,16 +5915,16 @@
         <v>225</v>
       </c>
       <c r="Q46" s="6" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="S46" s="31" t="s">
-        <v>247</v>
+        <v>270</v>
+      </c>
+      <c r="S46" s="6" t="s">
+        <v>294</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U46" s="8" t="s">
         <v>5</v>
@@ -5987,7 +5937,7 @@
         <v>151</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Z46" s="6" t="s">
         <v>200</v>
@@ -6011,14 +5961,14 @@
         <v>225</v>
       </c>
       <c r="AG46" s="6" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="AH46" s="6" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="AI46" s="6"/>
       <c r="AJ46" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="102" hidden="1" x14ac:dyDescent="0.2">
@@ -6155,7 +6105,7 @@
         <v>32</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>171</v>
@@ -6167,7 +6117,7 @@
         <v>210</v>
       </c>
       <c r="I49" s="56" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="J49" s="61" t="s">
         <v>190</v>
@@ -6191,16 +6141,16 @@
         <v>226</v>
       </c>
       <c r="Q49" s="6" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="R49" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="S49" s="70" t="s">
-        <v>248</v>
+        <v>277</v>
+      </c>
+      <c r="S49" s="61" t="s">
+        <v>297</v>
       </c>
       <c r="T49" s="61" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U49" s="8" t="s">
         <v>5</v>
@@ -6213,7 +6163,7 @@
         <v>166</v>
       </c>
       <c r="Y49" s="6" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="Z49" s="6" t="s">
         <v>189</v>
@@ -6237,14 +6187,14 @@
         <v>226</v>
       </c>
       <c r="AG49" s="6" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="AH49" s="6" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="AI49" s="6"/>
       <c r="AJ49" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:36" ht="119" hidden="1" x14ac:dyDescent="0.2">
@@ -6321,7 +6271,7 @@
         <v>31</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>85</v>
@@ -6333,7 +6283,7 @@
         <v>0.15548490000000001</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>192</v>
@@ -6357,16 +6307,16 @@
         <v>192</v>
       </c>
       <c r="Q51" s="61" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R51" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="S51" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="S51" s="6" t="s">
         <v>192</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U51" s="8" t="s">
         <v>3</v>
@@ -6379,7 +6329,7 @@
         <v>165</v>
       </c>
       <c r="Y51" s="6" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="Z51" s="6" t="s">
         <v>193</v>
@@ -6403,14 +6353,14 @@
         <v>193</v>
       </c>
       <c r="AG51" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="AH51" s="6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="AI51" s="6"/>
       <c r="AJ51" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:36" ht="51" x14ac:dyDescent="0.2">
@@ -6439,7 +6389,7 @@
         <v>0.15548490000000001</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>192</v>
@@ -6463,16 +6413,16 @@
         <v>192</v>
       </c>
       <c r="Q52" s="6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R52" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="S52" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="S52" s="6" t="s">
         <v>192</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U52" s="8" t="s">
         <v>3</v>
@@ -6485,7 +6435,7 @@
         <v>165</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="Z52" s="6" t="s">
         <v>193</v>
@@ -6509,7 +6459,7 @@
         <v>193</v>
       </c>
       <c r="AG52" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="AH52" s="6"/>
       <c r="AI52" s="6"/>
@@ -6529,7 +6479,7 @@
         <v>32</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>172</v>
@@ -6541,7 +6491,7 @@
         <v>168</v>
       </c>
       <c r="I53" s="56" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>214</v>
@@ -6565,16 +6515,16 @@
         <v>228</v>
       </c>
       <c r="Q53" s="6" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="R53" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="S53" s="31" t="s">
-        <v>231</v>
+        <v>283</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="T53" s="61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U53" s="8"/>
       <c r="V53" s="20"/>
@@ -6607,14 +6557,14 @@
         <v>227</v>
       </c>
       <c r="AG53" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="AH53" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="AI53" s="6"/>
       <c r="AJ53" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="119" hidden="1" x14ac:dyDescent="0.2">
@@ -6691,7 +6641,7 @@
         <v>31</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>85</v>
@@ -6703,7 +6653,7 @@
         <v>7.5484389999999998E-2</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J55" s="6" t="s">
         <v>195</v>
@@ -6727,16 +6677,16 @@
         <v>195</v>
       </c>
       <c r="Q55" s="6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="S55" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="S55" s="6" t="s">
         <v>195</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U55" s="8" t="s">
         <v>3</v>
@@ -6749,7 +6699,7 @@
         <v>175</v>
       </c>
       <c r="Y55" s="6" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="Z55" s="6" t="s">
         <v>196</v>
@@ -6773,14 +6723,14 @@
         <v>196</v>
       </c>
       <c r="AG55" s="6" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="AH55" s="6" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="AI55" s="6"/>
       <c r="AJ55" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:36" ht="51" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>